<commit_message>
Version 1.1.0.0 Public Beta
</commit_message>
<xml_diff>
--- a/MapLab3D_ProjectParameters_1_1_0_0_Colors_Database.xlsx
+++ b/MapLab3D_ProjectParameters_1_1_0_0_Colors_Database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Daten\Projekte\MapLab3D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B09AA4-79B0-40C3-B27B-BCE4EC48E7E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DB998E-42CD-456A-BF25-EA0B6E91C8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4740" windowWidth="8070" windowHeight="7710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="210" windowWidth="24180" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,26 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7659" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7660" uniqueCount="332">
   <si>
     <t>N</t>
   </si>
@@ -604,9 +618,6 @@
     <t>https://www.conrad.de/de/p/verbatim-55050-filament-petg-1-75-mm-1-kg-weiss-1-st-1969823.html</t>
   </si>
   <si>
-    <t>https://shop.fillamentum.com/collections/pla-extrafill-filament/products/fillamentum-pla-extrafill-cobalt-blue</t>
-  </si>
-  <si>
     <t>Cobalt Blue</t>
   </si>
   <si>
@@ -1023,12 +1034,18 @@
   <si>
     <t>Green</t>
   </si>
+  <si>
+    <t>https://shop.fillamentum.com/collections/pla-extrafill-filament/products/pla-extrafill-cobalt-blue-1kg</t>
+  </si>
+  <si>
+    <t>RAL 5013</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1088,6 +1105,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="83">
@@ -2283,12 +2308,6 @@
     <xf numFmtId="0" fontId="7" fillId="51" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="45" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="45" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="46" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2508,6 +2527,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="82" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="45" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="45" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="77" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2815,8 +2840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1295"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A718" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z726" sqref="Z726"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2834,14 +2859,14 @@
     <col min="12" max="14" width="2.42578125" style="11" customWidth="1"/>
     <col min="15" max="15" width="30.28515625" style="11" customWidth="1"/>
     <col min="16" max="17" width="2.42578125" style="11" customWidth="1"/>
-    <col min="18" max="18" width="38.28515625" style="225" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="38.28515625" style="223" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="2.7109375" style="11" customWidth="1"/>
     <col min="20" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="236" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B1" s="237"/>
       <c r="C1" s="237"/>
@@ -2863,7 +2888,7 @@
     </row>
     <row r="2" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="236" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B2" s="237"/>
       <c r="C2" s="237"/>
@@ -2885,7 +2910,7 @@
     </row>
     <row r="3" spans="1:18" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="236" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B3" s="237"/>
       <c r="C3" s="237"/>
@@ -3166,7 +3191,7 @@
       <c r="M10" s="40"/>
       <c r="N10" s="37"/>
       <c r="O10" s="42" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="44" t="s">
@@ -4174,7 +4199,7 @@
       <c r="M36" s="40"/>
       <c r="N36" s="37"/>
       <c r="O36" s="63" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="P36" s="10"/>
       <c r="Q36" s="44" t="s">
@@ -13740,7 +13765,7 @@
       <c r="M283" s="40"/>
       <c r="N283" s="37"/>
       <c r="O283" s="114" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="P283" s="10"/>
       <c r="Q283" s="44" t="s">
@@ -13970,7 +13995,7 @@
       <c r="M289" s="54"/>
       <c r="N289" s="55"/>
       <c r="O289" s="115" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P289" s="52"/>
       <c r="Q289" s="57" t="s">
@@ -19874,7 +19899,7 @@
       <c r="M443" s="40"/>
       <c r="N443" s="37"/>
       <c r="O443" s="123" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P443" s="10"/>
       <c r="Q443" s="44" t="s">
@@ -19913,7 +19938,7 @@
       <c r="M444" s="40"/>
       <c r="N444" s="37"/>
       <c r="O444" s="123" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P444" s="10"/>
       <c r="Q444" s="44" t="s">
@@ -24642,7 +24667,7 @@
       <c r="L566" s="30"/>
       <c r="M566" s="80"/>
       <c r="N566" s="37"/>
-      <c r="O566" s="230">
+      <c r="O566" s="228">
         <v>174</v>
       </c>
       <c r="P566" s="10"/>
@@ -24683,7 +24708,7 @@
       <c r="L567" s="30"/>
       <c r="M567" s="80"/>
       <c r="N567" s="37"/>
-      <c r="O567" s="230">
+      <c r="O567" s="228">
         <v>174</v>
       </c>
       <c r="P567" s="10"/>
@@ -24724,7 +24749,7 @@
       <c r="L568" s="30"/>
       <c r="M568" s="80"/>
       <c r="N568" s="37"/>
-      <c r="O568" s="230">
+      <c r="O568" s="228">
         <v>174</v>
       </c>
       <c r="P568" s="10"/>
@@ -24761,7 +24786,7 @@
       <c r="L569" s="10"/>
       <c r="M569" s="40"/>
       <c r="N569" s="37"/>
-      <c r="O569" s="230" t="s">
+      <c r="O569" s="228" t="s">
         <v>99</v>
       </c>
       <c r="P569" s="10"/>
@@ -24800,7 +24825,7 @@
       <c r="L570" s="10"/>
       <c r="M570" s="40"/>
       <c r="N570" s="37"/>
-      <c r="O570" s="230"/>
+      <c r="O570" s="228"/>
       <c r="P570" s="10"/>
       <c r="Q570" s="44" t="s">
         <v>15</v>
@@ -24837,7 +24862,7 @@
       <c r="L571" s="10"/>
       <c r="M571" s="40"/>
       <c r="N571" s="37"/>
-      <c r="O571" s="230" t="s">
+      <c r="O571" s="228" t="s">
         <v>101</v>
       </c>
       <c r="P571" s="10"/>
@@ -24876,7 +24901,7 @@
       <c r="L572" s="10"/>
       <c r="M572" s="40"/>
       <c r="N572" s="37"/>
-      <c r="O572" s="230" t="s">
+      <c r="O572" s="228" t="s">
         <v>23</v>
       </c>
       <c r="P572" s="10"/>
@@ -24915,7 +24940,7 @@
       <c r="L573" s="10"/>
       <c r="M573" s="40"/>
       <c r="N573" s="37"/>
-      <c r="O573" s="230" t="s">
+      <c r="O573" s="228" t="s">
         <v>43</v>
       </c>
       <c r="P573" s="10"/>
@@ -24954,7 +24979,7 @@
       <c r="L574" s="10"/>
       <c r="M574" s="40"/>
       <c r="N574" s="37"/>
-      <c r="O574" s="230" t="s">
+      <c r="O574" s="228" t="s">
         <v>44</v>
       </c>
       <c r="P574" s="10"/>
@@ -24993,7 +25018,7 @@
       <c r="L575" s="52"/>
       <c r="M575" s="54"/>
       <c r="N575" s="55"/>
-      <c r="O575" s="231" t="s">
+      <c r="O575" s="229" t="s">
         <v>103</v>
       </c>
       <c r="P575" s="52"/>
@@ -27008,7 +27033,7 @@
       <c r="M627" s="54"/>
       <c r="N627" s="55"/>
       <c r="O627" s="147" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P627" s="52"/>
       <c r="Q627" s="57" t="s">
@@ -28792,7 +28817,7 @@
       <c r="M673" s="40"/>
       <c r="N673" s="37"/>
       <c r="O673" s="151" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="P673" s="10"/>
       <c r="Q673" s="44" t="s">
@@ -29022,7 +29047,7 @@
       <c r="M679" s="54"/>
       <c r="N679" s="55"/>
       <c r="O679" s="152" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P679" s="52"/>
       <c r="Q679" s="57" t="s">
@@ -30800,7 +30825,7 @@
       <c r="M725" s="40"/>
       <c r="N725" s="37"/>
       <c r="O725" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P725" s="10"/>
       <c r="Q725" s="44" t="s">
@@ -31030,7 +31055,7 @@
       <c r="M731" s="54"/>
       <c r="N731" s="55"/>
       <c r="O731" s="159" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P731" s="52"/>
       <c r="Q731" s="57" t="s">
@@ -31182,7 +31207,7 @@
       <c r="L735" s="30"/>
       <c r="M735" s="80"/>
       <c r="N735" s="37"/>
-      <c r="O735" s="160">
+      <c r="O735" s="234">
         <v>47</v>
       </c>
       <c r="P735" s="10"/>
@@ -31223,7 +31248,7 @@
       <c r="L736" s="30"/>
       <c r="M736" s="80"/>
       <c r="N736" s="37"/>
-      <c r="O736" s="160">
+      <c r="O736" s="234">
         <v>67</v>
       </c>
       <c r="P736" s="10"/>
@@ -31264,7 +31289,7 @@
       <c r="L737" s="30"/>
       <c r="M737" s="80"/>
       <c r="N737" s="37"/>
-      <c r="O737" s="160">
+      <c r="O737" s="234">
         <v>124</v>
       </c>
       <c r="P737" s="10"/>
@@ -31301,8 +31326,8 @@
       <c r="L738" s="10"/>
       <c r="M738" s="40"/>
       <c r="N738" s="37"/>
-      <c r="O738" s="160" t="s">
-        <v>192</v>
+      <c r="O738" s="234" t="s">
+        <v>191</v>
       </c>
       <c r="P738" s="10"/>
       <c r="Q738" s="44" t="s">
@@ -31340,7 +31365,9 @@
       <c r="L739" s="10"/>
       <c r="M739" s="40"/>
       <c r="N739" s="37"/>
-      <c r="O739" s="160"/>
+      <c r="O739" s="234" t="s">
+        <v>331</v>
+      </c>
       <c r="P739" s="10"/>
       <c r="Q739" s="44" t="s">
         <v>15</v>
@@ -31377,7 +31404,7 @@
       <c r="L740" s="10"/>
       <c r="M740" s="40"/>
       <c r="N740" s="37"/>
-      <c r="O740" s="160"/>
+      <c r="O740" s="234"/>
       <c r="P740" s="10"/>
       <c r="Q740" s="44" t="s">
         <v>15</v>
@@ -31414,7 +31441,7 @@
       <c r="L741" s="10"/>
       <c r="M741" s="40"/>
       <c r="N741" s="37"/>
-      <c r="O741" s="160" t="s">
+      <c r="O741" s="234" t="s">
         <v>23</v>
       </c>
       <c r="P741" s="10"/>
@@ -31453,7 +31480,7 @@
       <c r="L742" s="10"/>
       <c r="M742" s="40"/>
       <c r="N742" s="37"/>
-      <c r="O742" s="160" t="s">
+      <c r="O742" s="234" t="s">
         <v>28</v>
       </c>
       <c r="P742" s="10"/>
@@ -31492,7 +31519,7 @@
       <c r="L743" s="10"/>
       <c r="M743" s="40"/>
       <c r="N743" s="37"/>
-      <c r="O743" s="160" t="s">
+      <c r="O743" s="234" t="s">
         <v>31</v>
       </c>
       <c r="P743" s="10"/>
@@ -31503,7 +31530,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="744" spans="1:18" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="744" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="A744" s="46" t="s">
         <v>2</v>
       </c>
@@ -31531,8 +31558,8 @@
       <c r="L744" s="52"/>
       <c r="M744" s="54"/>
       <c r="N744" s="55"/>
-      <c r="O744" s="161" t="s">
-        <v>191</v>
+      <c r="O744" s="235" t="s">
+        <v>330</v>
       </c>
       <c r="P744" s="52"/>
       <c r="Q744" s="57" t="s">
@@ -31684,7 +31711,7 @@
       <c r="L748" s="30"/>
       <c r="M748" s="80"/>
       <c r="N748" s="37"/>
-      <c r="O748" s="162">
+      <c r="O748" s="160">
         <v>0</v>
       </c>
       <c r="P748" s="10"/>
@@ -31725,7 +31752,7 @@
       <c r="L749" s="30"/>
       <c r="M749" s="80"/>
       <c r="N749" s="37"/>
-      <c r="O749" s="162">
+      <c r="O749" s="160">
         <v>106</v>
       </c>
       <c r="P749" s="10"/>
@@ -31766,7 +31793,7 @@
       <c r="L750" s="30"/>
       <c r="M750" s="80"/>
       <c r="N750" s="37"/>
-      <c r="O750" s="162">
+      <c r="O750" s="160">
         <v>92</v>
       </c>
       <c r="P750" s="10"/>
@@ -31803,8 +31830,8 @@
       <c r="L751" s="10"/>
       <c r="M751" s="40"/>
       <c r="N751" s="37"/>
-      <c r="O751" s="162" t="s">
-        <v>194</v>
+      <c r="O751" s="160" t="s">
+        <v>193</v>
       </c>
       <c r="P751" s="10"/>
       <c r="Q751" s="44" t="s">
@@ -31842,7 +31869,7 @@
       <c r="L752" s="10"/>
       <c r="M752" s="40"/>
       <c r="N752" s="37"/>
-      <c r="O752" s="162"/>
+      <c r="O752" s="160"/>
       <c r="P752" s="10"/>
       <c r="Q752" s="44" t="s">
         <v>15</v>
@@ -31879,8 +31906,8 @@
       <c r="L753" s="10"/>
       <c r="M753" s="40"/>
       <c r="N753" s="37"/>
-      <c r="O753" s="162" t="s">
-        <v>195</v>
+      <c r="O753" s="160" t="s">
+        <v>194</v>
       </c>
       <c r="P753" s="10"/>
       <c r="Q753" s="44" t="s">
@@ -31918,7 +31945,7 @@
       <c r="L754" s="10"/>
       <c r="M754" s="40"/>
       <c r="N754" s="37"/>
-      <c r="O754" s="162" t="s">
+      <c r="O754" s="160" t="s">
         <v>23</v>
       </c>
       <c r="P754" s="10"/>
@@ -31957,8 +31984,8 @@
       <c r="L755" s="10"/>
       <c r="M755" s="40"/>
       <c r="N755" s="37"/>
-      <c r="O755" s="162" t="s">
-        <v>196</v>
+      <c r="O755" s="160" t="s">
+        <v>195</v>
       </c>
       <c r="P755" s="10"/>
       <c r="Q755" s="44" t="s">
@@ -31996,8 +32023,8 @@
       <c r="L756" s="10"/>
       <c r="M756" s="40"/>
       <c r="N756" s="37"/>
-      <c r="O756" s="162" t="s">
-        <v>197</v>
+      <c r="O756" s="160" t="s">
+        <v>196</v>
       </c>
       <c r="P756" s="10"/>
       <c r="Q756" s="44" t="s">
@@ -32035,8 +32062,8 @@
       <c r="L757" s="52"/>
       <c r="M757" s="54"/>
       <c r="N757" s="55"/>
-      <c r="O757" s="163" t="s">
-        <v>198</v>
+      <c r="O757" s="161" t="s">
+        <v>197</v>
       </c>
       <c r="P757" s="52"/>
       <c r="Q757" s="57" t="s">
@@ -32529,7 +32556,7 @@
       <c r="L770" s="52"/>
       <c r="M770" s="54"/>
       <c r="N770" s="55"/>
-      <c r="O770" s="164"/>
+      <c r="O770" s="162"/>
       <c r="P770" s="52"/>
       <c r="Q770" s="57" t="s">
         <v>15</v>
@@ -33031,7 +33058,7 @@
       <c r="L783" s="52"/>
       <c r="M783" s="54"/>
       <c r="N783" s="55"/>
-      <c r="O783" s="165" t="s">
+      <c r="O783" s="163" t="s">
         <v>185</v>
       </c>
       <c r="P783" s="52"/>
@@ -33184,7 +33211,7 @@
       <c r="L787" s="30"/>
       <c r="M787" s="80"/>
       <c r="N787" s="37"/>
-      <c r="O787" s="166">
+      <c r="O787" s="164">
         <v>255</v>
       </c>
       <c r="P787" s="10"/>
@@ -33225,7 +33252,7 @@
       <c r="L788" s="30"/>
       <c r="M788" s="80"/>
       <c r="N788" s="37"/>
-      <c r="O788" s="166">
+      <c r="O788" s="164">
         <v>0</v>
       </c>
       <c r="P788" s="10"/>
@@ -33266,7 +33293,7 @@
       <c r="L789" s="30"/>
       <c r="M789" s="80"/>
       <c r="N789" s="37"/>
-      <c r="O789" s="166">
+      <c r="O789" s="164">
         <v>0</v>
       </c>
       <c r="P789" s="10"/>
@@ -33303,7 +33330,7 @@
       <c r="L790" s="10"/>
       <c r="M790" s="40"/>
       <c r="N790" s="37"/>
-      <c r="O790" s="166" t="s">
+      <c r="O790" s="164" t="s">
         <v>105</v>
       </c>
       <c r="P790" s="10"/>
@@ -33342,7 +33369,7 @@
       <c r="L791" s="10"/>
       <c r="M791" s="40"/>
       <c r="N791" s="37"/>
-      <c r="O791" s="166"/>
+      <c r="O791" s="164"/>
       <c r="P791" s="10"/>
       <c r="Q791" s="44" t="s">
         <v>15</v>
@@ -33379,7 +33406,7 @@
       <c r="L792" s="10"/>
       <c r="M792" s="40"/>
       <c r="N792" s="37"/>
-      <c r="O792" s="166" t="s">
+      <c r="O792" s="164" t="s">
         <v>186</v>
       </c>
       <c r="P792" s="10"/>
@@ -33418,7 +33445,7 @@
       <c r="L793" s="10"/>
       <c r="M793" s="40"/>
       <c r="N793" s="37"/>
-      <c r="O793" s="166" t="s">
+      <c r="O793" s="164" t="s">
         <v>155</v>
       </c>
       <c r="P793" s="10"/>
@@ -33457,7 +33484,7 @@
       <c r="L794" s="10"/>
       <c r="M794" s="40"/>
       <c r="N794" s="37"/>
-      <c r="O794" s="166" t="s">
+      <c r="O794" s="164" t="s">
         <v>26</v>
       </c>
       <c r="P794" s="10"/>
@@ -33496,7 +33523,7 @@
       <c r="L795" s="10"/>
       <c r="M795" s="40"/>
       <c r="N795" s="37"/>
-      <c r="O795" s="166" t="s">
+      <c r="O795" s="164" t="s">
         <v>26</v>
       </c>
       <c r="P795" s="10"/>
@@ -33535,7 +33562,7 @@
       <c r="L796" s="52"/>
       <c r="M796" s="54"/>
       <c r="N796" s="55"/>
-      <c r="O796" s="167" t="s">
+      <c r="O796" s="165" t="s">
         <v>187</v>
       </c>
       <c r="P796" s="52"/>
@@ -33688,7 +33715,7 @@
       <c r="L800" s="30"/>
       <c r="M800" s="80"/>
       <c r="N800" s="37"/>
-      <c r="O800" s="168">
+      <c r="O800" s="166">
         <v>249</v>
       </c>
       <c r="P800" s="10"/>
@@ -33729,7 +33756,7 @@
       <c r="L801" s="30"/>
       <c r="M801" s="80"/>
       <c r="N801" s="37"/>
-      <c r="O801" s="168">
+      <c r="O801" s="166">
         <v>249</v>
       </c>
       <c r="P801" s="10"/>
@@ -33770,7 +33797,7 @@
       <c r="L802" s="30"/>
       <c r="M802" s="80"/>
       <c r="N802" s="37"/>
-      <c r="O802" s="168">
+      <c r="O802" s="166">
         <v>249</v>
       </c>
       <c r="P802" s="10"/>
@@ -33807,7 +33834,7 @@
       <c r="L803" s="10"/>
       <c r="M803" s="40"/>
       <c r="N803" s="37"/>
-      <c r="O803" s="168" t="s">
+      <c r="O803" s="166" t="s">
         <v>188</v>
       </c>
       <c r="P803" s="10"/>
@@ -33846,7 +33873,7 @@
       <c r="L804" s="10"/>
       <c r="M804" s="40"/>
       <c r="N804" s="37"/>
-      <c r="O804" s="168"/>
+      <c r="O804" s="166"/>
       <c r="P804" s="10"/>
       <c r="Q804" s="44" t="s">
         <v>15</v>
@@ -33883,7 +33910,7 @@
       <c r="L805" s="10"/>
       <c r="M805" s="40"/>
       <c r="N805" s="37"/>
-      <c r="O805" s="168" t="s">
+      <c r="O805" s="166" t="s">
         <v>189</v>
       </c>
       <c r="P805" s="10"/>
@@ -33922,7 +33949,7 @@
       <c r="L806" s="10"/>
       <c r="M806" s="40"/>
       <c r="N806" s="37"/>
-      <c r="O806" s="168" t="s">
+      <c r="O806" s="166" t="s">
         <v>155</v>
       </c>
       <c r="P806" s="10"/>
@@ -33961,7 +33988,7 @@
       <c r="L807" s="10"/>
       <c r="M807" s="40"/>
       <c r="N807" s="37"/>
-      <c r="O807" s="168" t="s">
+      <c r="O807" s="166" t="s">
         <v>26</v>
       </c>
       <c r="P807" s="10"/>
@@ -34000,7 +34027,7 @@
       <c r="L808" s="10"/>
       <c r="M808" s="40"/>
       <c r="N808" s="37"/>
-      <c r="O808" s="168" t="s">
+      <c r="O808" s="166" t="s">
         <v>26</v>
       </c>
       <c r="P808" s="10"/>
@@ -34039,7 +34066,7 @@
       <c r="L809" s="52"/>
       <c r="M809" s="54"/>
       <c r="N809" s="55"/>
-      <c r="O809" s="169" t="s">
+      <c r="O809" s="167" t="s">
         <v>190</v>
       </c>
       <c r="P809" s="52"/>
@@ -34192,7 +34219,7 @@
       <c r="L813" s="30"/>
       <c r="M813" s="80"/>
       <c r="N813" s="37"/>
-      <c r="O813" s="232">
+      <c r="O813" s="230">
         <v>146</v>
       </c>
       <c r="P813" s="10"/>
@@ -34233,7 +34260,7 @@
       <c r="L814" s="30"/>
       <c r="M814" s="80"/>
       <c r="N814" s="37"/>
-      <c r="O814" s="232">
+      <c r="O814" s="230">
         <v>106</v>
       </c>
       <c r="P814" s="10"/>
@@ -34274,7 +34301,7 @@
       <c r="L815" s="30"/>
       <c r="M815" s="80"/>
       <c r="N815" s="37"/>
-      <c r="O815" s="232">
+      <c r="O815" s="230">
         <v>166</v>
       </c>
       <c r="P815" s="10"/>
@@ -34311,8 +34338,8 @@
       <c r="L816" s="10"/>
       <c r="M816" s="40"/>
       <c r="N816" s="37"/>
-      <c r="O816" s="232" t="s">
-        <v>207</v>
+      <c r="O816" s="230" t="s">
+        <v>206</v>
       </c>
       <c r="P816" s="10"/>
       <c r="Q816" s="44" t="s">
@@ -34350,7 +34377,7 @@
       <c r="L817" s="10"/>
       <c r="M817" s="40"/>
       <c r="N817" s="37"/>
-      <c r="O817" s="232"/>
+      <c r="O817" s="230"/>
       <c r="P817" s="10"/>
       <c r="Q817" s="44" t="s">
         <v>15</v>
@@ -34387,8 +34414,8 @@
       <c r="L818" s="10"/>
       <c r="M818" s="40"/>
       <c r="N818" s="37"/>
-      <c r="O818" s="232" t="s">
-        <v>209</v>
+      <c r="O818" s="230" t="s">
+        <v>208</v>
       </c>
       <c r="P818" s="10"/>
       <c r="Q818" s="44" t="s">
@@ -34426,7 +34453,7 @@
       <c r="L819" s="10"/>
       <c r="M819" s="40"/>
       <c r="N819" s="37"/>
-      <c r="O819" s="232" t="s">
+      <c r="O819" s="230" t="s">
         <v>23</v>
       </c>
       <c r="P819" s="10"/>
@@ -34465,8 +34492,8 @@
       <c r="L820" s="10"/>
       <c r="M820" s="40"/>
       <c r="N820" s="37"/>
-      <c r="O820" s="232" t="s">
-        <v>206</v>
+      <c r="O820" s="230" t="s">
+        <v>205</v>
       </c>
       <c r="P820" s="10"/>
       <c r="Q820" s="44" t="s">
@@ -34504,8 +34531,8 @@
       <c r="L821" s="10"/>
       <c r="M821" s="40"/>
       <c r="N821" s="37"/>
-      <c r="O821" s="232" t="s">
-        <v>208</v>
+      <c r="O821" s="230" t="s">
+        <v>207</v>
       </c>
       <c r="P821" s="10"/>
       <c r="Q821" s="44" t="s">
@@ -34543,8 +34570,8 @@
       <c r="L822" s="52"/>
       <c r="M822" s="54"/>
       <c r="N822" s="55"/>
-      <c r="O822" s="233" t="s">
-        <v>210</v>
+      <c r="O822" s="231" t="s">
+        <v>209</v>
       </c>
       <c r="P822" s="52"/>
       <c r="Q822" s="57" t="s">
@@ -34696,7 +34723,7 @@
       <c r="L826" s="30"/>
       <c r="M826" s="80"/>
       <c r="N826" s="37"/>
-      <c r="O826" s="170">
+      <c r="O826" s="168">
         <v>169</v>
       </c>
       <c r="P826" s="10"/>
@@ -34737,7 +34764,7 @@
       <c r="L827" s="30"/>
       <c r="M827" s="80"/>
       <c r="N827" s="37"/>
-      <c r="O827" s="170">
+      <c r="O827" s="168">
         <v>133</v>
       </c>
       <c r="P827" s="10"/>
@@ -34778,7 +34805,7 @@
       <c r="L828" s="30"/>
       <c r="M828" s="80"/>
       <c r="N828" s="37"/>
-      <c r="O828" s="170">
+      <c r="O828" s="168">
         <v>221</v>
       </c>
       <c r="P828" s="10"/>
@@ -34815,8 +34842,8 @@
       <c r="L829" s="10"/>
       <c r="M829" s="40"/>
       <c r="N829" s="37"/>
-      <c r="O829" s="170" t="s">
-        <v>212</v>
+      <c r="O829" s="168" t="s">
+        <v>211</v>
       </c>
       <c r="P829" s="10"/>
       <c r="Q829" s="44" t="s">
@@ -34854,7 +34881,7 @@
       <c r="L830" s="10"/>
       <c r="M830" s="40"/>
       <c r="N830" s="37"/>
-      <c r="O830" s="170"/>
+      <c r="O830" s="168"/>
       <c r="P830" s="10"/>
       <c r="Q830" s="44" t="s">
         <v>15</v>
@@ -34891,8 +34918,8 @@
       <c r="L831" s="10"/>
       <c r="M831" s="40"/>
       <c r="N831" s="37"/>
-      <c r="O831" s="170" t="s">
-        <v>213</v>
+      <c r="O831" s="168" t="s">
+        <v>212</v>
       </c>
       <c r="P831" s="10"/>
       <c r="Q831" s="44" t="s">
@@ -34930,7 +34957,7 @@
       <c r="L832" s="10"/>
       <c r="M832" s="40"/>
       <c r="N832" s="37"/>
-      <c r="O832" s="170" t="s">
+      <c r="O832" s="168" t="s">
         <v>23</v>
       </c>
       <c r="P832" s="10"/>
@@ -34969,8 +34996,8 @@
       <c r="L833" s="10"/>
       <c r="M833" s="40"/>
       <c r="N833" s="37"/>
-      <c r="O833" s="170" t="s">
-        <v>214</v>
+      <c r="O833" s="168" t="s">
+        <v>213</v>
       </c>
       <c r="P833" s="10"/>
       <c r="Q833" s="44" t="s">
@@ -35008,8 +35035,8 @@
       <c r="L834" s="10"/>
       <c r="M834" s="40"/>
       <c r="N834" s="37"/>
-      <c r="O834" s="170" t="s">
-        <v>211</v>
+      <c r="O834" s="168" t="s">
+        <v>210</v>
       </c>
       <c r="P834" s="10"/>
       <c r="Q834" s="44" t="s">
@@ -35047,8 +35074,8 @@
       <c r="L835" s="52"/>
       <c r="M835" s="54"/>
       <c r="N835" s="55"/>
-      <c r="O835" s="171" t="s">
-        <v>215</v>
+      <c r="O835" s="169" t="s">
+        <v>214</v>
       </c>
       <c r="P835" s="52"/>
       <c r="Q835" s="57" t="s">
@@ -35200,7 +35227,7 @@
       <c r="L839" s="30"/>
       <c r="M839" s="80"/>
       <c r="N839" s="37"/>
-      <c r="O839" s="172">
+      <c r="O839" s="170">
         <v>199</v>
       </c>
       <c r="P839" s="10"/>
@@ -35241,7 +35268,7 @@
       <c r="L840" s="30"/>
       <c r="M840" s="80"/>
       <c r="N840" s="37"/>
-      <c r="O840" s="172">
+      <c r="O840" s="170">
         <v>174</v>
       </c>
       <c r="P840" s="10"/>
@@ -35282,7 +35309,7 @@
       <c r="L841" s="30"/>
       <c r="M841" s="80"/>
       <c r="N841" s="37"/>
-      <c r="O841" s="172">
+      <c r="O841" s="170">
         <v>207</v>
       </c>
       <c r="P841" s="10"/>
@@ -35319,8 +35346,8 @@
       <c r="L842" s="10"/>
       <c r="M842" s="40"/>
       <c r="N842" s="37"/>
-      <c r="O842" s="172" t="s">
-        <v>216</v>
+      <c r="O842" s="170" t="s">
+        <v>215</v>
       </c>
       <c r="P842" s="10"/>
       <c r="Q842" s="44" t="s">
@@ -35358,7 +35385,7 @@
       <c r="L843" s="10"/>
       <c r="M843" s="40"/>
       <c r="N843" s="37"/>
-      <c r="O843" s="172"/>
+      <c r="O843" s="170"/>
       <c r="P843" s="10"/>
       <c r="Q843" s="44" t="s">
         <v>15</v>
@@ -35395,8 +35422,8 @@
       <c r="L844" s="10"/>
       <c r="M844" s="40"/>
       <c r="N844" s="37"/>
-      <c r="O844" s="172" t="s">
-        <v>217</v>
+      <c r="O844" s="170" t="s">
+        <v>216</v>
       </c>
       <c r="P844" s="10"/>
       <c r="Q844" s="44" t="s">
@@ -35434,7 +35461,7 @@
       <c r="L845" s="10"/>
       <c r="M845" s="40"/>
       <c r="N845" s="37"/>
-      <c r="O845" s="172" t="s">
+      <c r="O845" s="170" t="s">
         <v>23</v>
       </c>
       <c r="P845" s="10"/>
@@ -35473,8 +35500,8 @@
       <c r="L846" s="10"/>
       <c r="M846" s="40"/>
       <c r="N846" s="37"/>
-      <c r="O846" s="172" t="s">
-        <v>206</v>
+      <c r="O846" s="170" t="s">
+        <v>205</v>
       </c>
       <c r="P846" s="10"/>
       <c r="Q846" s="44" t="s">
@@ -35512,8 +35539,8 @@
       <c r="L847" s="10"/>
       <c r="M847" s="40"/>
       <c r="N847" s="37"/>
-      <c r="O847" s="172" t="s">
-        <v>208</v>
+      <c r="O847" s="170" t="s">
+        <v>207</v>
       </c>
       <c r="P847" s="10"/>
       <c r="Q847" s="44" t="s">
@@ -35551,8 +35578,8 @@
       <c r="L848" s="52"/>
       <c r="M848" s="54"/>
       <c r="N848" s="55"/>
-      <c r="O848" s="173" t="s">
-        <v>218</v>
+      <c r="O848" s="171" t="s">
+        <v>217</v>
       </c>
       <c r="P848" s="52"/>
       <c r="Q848" s="57" t="s">
@@ -35704,7 +35731,7 @@
       <c r="L852" s="30"/>
       <c r="M852" s="80"/>
       <c r="N852" s="37"/>
-      <c r="O852" s="234">
+      <c r="O852" s="232">
         <v>200</v>
       </c>
       <c r="P852" s="10"/>
@@ -35745,7 +35772,7 @@
       <c r="L853" s="30"/>
       <c r="M853" s="80"/>
       <c r="N853" s="37"/>
-      <c r="O853" s="234">
+      <c r="O853" s="232">
         <v>48</v>
       </c>
       <c r="P853" s="10"/>
@@ -35786,7 +35813,7 @@
       <c r="L854" s="30"/>
       <c r="M854" s="80"/>
       <c r="N854" s="37"/>
-      <c r="O854" s="234">
+      <c r="O854" s="232">
         <v>123</v>
       </c>
       <c r="P854" s="10"/>
@@ -35823,8 +35850,8 @@
       <c r="L855" s="10"/>
       <c r="M855" s="40"/>
       <c r="N855" s="37"/>
-      <c r="O855" s="234" t="s">
-        <v>219</v>
+      <c r="O855" s="232" t="s">
+        <v>218</v>
       </c>
       <c r="P855" s="10"/>
       <c r="Q855" s="44" t="s">
@@ -35862,8 +35889,8 @@
       <c r="L856" s="10"/>
       <c r="M856" s="40"/>
       <c r="N856" s="37"/>
-      <c r="O856" s="234" t="s">
-        <v>222</v>
+      <c r="O856" s="232" t="s">
+        <v>221</v>
       </c>
       <c r="P856" s="10"/>
       <c r="Q856" s="44" t="s">
@@ -35901,8 +35928,8 @@
       <c r="L857" s="10"/>
       <c r="M857" s="40"/>
       <c r="N857" s="37"/>
-      <c r="O857" s="234" t="s">
-        <v>220</v>
+      <c r="O857" s="232" t="s">
+        <v>219</v>
       </c>
       <c r="P857" s="10"/>
       <c r="Q857" s="44" t="s">
@@ -35940,7 +35967,7 @@
       <c r="L858" s="10"/>
       <c r="M858" s="40"/>
       <c r="N858" s="37"/>
-      <c r="O858" s="234" t="s">
+      <c r="O858" s="232" t="s">
         <v>23</v>
       </c>
       <c r="P858" s="10"/>
@@ -35979,7 +36006,7 @@
       <c r="L859" s="10"/>
       <c r="M859" s="40"/>
       <c r="N859" s="37"/>
-      <c r="O859" s="234" t="s">
+      <c r="O859" s="232" t="s">
         <v>28</v>
       </c>
       <c r="P859" s="10"/>
@@ -36018,7 +36045,7 @@
       <c r="L860" s="10"/>
       <c r="M860" s="40"/>
       <c r="N860" s="37"/>
-      <c r="O860" s="234" t="s">
+      <c r="O860" s="232" t="s">
         <v>31</v>
       </c>
       <c r="P860" s="10"/>
@@ -36057,8 +36084,8 @@
       <c r="L861" s="52"/>
       <c r="M861" s="54"/>
       <c r="N861" s="55"/>
-      <c r="O861" s="235" t="s">
-        <v>221</v>
+      <c r="O861" s="233" t="s">
+        <v>220</v>
       </c>
       <c r="P861" s="52"/>
       <c r="Q861" s="57" t="s">
@@ -36210,7 +36237,7 @@
       <c r="L865" s="30"/>
       <c r="M865" s="80"/>
       <c r="N865" s="37"/>
-      <c r="O865" s="174">
+      <c r="O865" s="172">
         <v>207</v>
       </c>
       <c r="P865" s="10"/>
@@ -36251,7 +36278,7 @@
       <c r="L866" s="30"/>
       <c r="M866" s="80"/>
       <c r="N866" s="37"/>
-      <c r="O866" s="174">
+      <c r="O866" s="172">
         <v>203</v>
       </c>
       <c r="P866" s="10"/>
@@ -36292,7 +36319,7 @@
       <c r="L867" s="30"/>
       <c r="M867" s="80"/>
       <c r="N867" s="37"/>
-      <c r="O867" s="174">
+      <c r="O867" s="172">
         <v>183</v>
       </c>
       <c r="P867" s="10"/>
@@ -36329,8 +36356,8 @@
       <c r="L868" s="10"/>
       <c r="M868" s="40"/>
       <c r="N868" s="37"/>
-      <c r="O868" s="174" t="s">
-        <v>223</v>
+      <c r="O868" s="172" t="s">
+        <v>222</v>
       </c>
       <c r="P868" s="10"/>
       <c r="Q868" s="44" t="s">
@@ -36368,8 +36395,8 @@
       <c r="L869" s="10"/>
       <c r="M869" s="40"/>
       <c r="N869" s="37"/>
-      <c r="O869" s="174" t="s">
-        <v>224</v>
+      <c r="O869" s="172" t="s">
+        <v>223</v>
       </c>
       <c r="P869" s="10"/>
       <c r="Q869" s="44" t="s">
@@ -36407,8 +36434,8 @@
       <c r="L870" s="10"/>
       <c r="M870" s="40"/>
       <c r="N870" s="37"/>
-      <c r="O870" s="174" t="s">
-        <v>225</v>
+      <c r="O870" s="172" t="s">
+        <v>224</v>
       </c>
       <c r="P870" s="10"/>
       <c r="Q870" s="44" t="s">
@@ -36446,7 +36473,7 @@
       <c r="L871" s="10"/>
       <c r="M871" s="40"/>
       <c r="N871" s="37"/>
-      <c r="O871" s="174" t="s">
+      <c r="O871" s="172" t="s">
         <v>23</v>
       </c>
       <c r="P871" s="10"/>
@@ -36485,7 +36512,7 @@
       <c r="L872" s="10"/>
       <c r="M872" s="40"/>
       <c r="N872" s="37"/>
-      <c r="O872" s="174" t="s">
+      <c r="O872" s="172" t="s">
         <v>28</v>
       </c>
       <c r="P872" s="10"/>
@@ -36524,7 +36551,7 @@
       <c r="L873" s="10"/>
       <c r="M873" s="40"/>
       <c r="N873" s="37"/>
-      <c r="O873" s="174" t="s">
+      <c r="O873" s="172" t="s">
         <v>31</v>
       </c>
       <c r="P873" s="10"/>
@@ -36563,8 +36590,8 @@
       <c r="L874" s="52"/>
       <c r="M874" s="54"/>
       <c r="N874" s="55"/>
-      <c r="O874" s="175" t="s">
-        <v>226</v>
+      <c r="O874" s="173" t="s">
+        <v>225</v>
       </c>
       <c r="P874" s="52"/>
       <c r="Q874" s="57" t="s">
@@ -36716,7 +36743,7 @@
       <c r="L878" s="30"/>
       <c r="M878" s="80"/>
       <c r="N878" s="37"/>
-      <c r="O878" s="176">
+      <c r="O878" s="174">
         <v>219</v>
       </c>
       <c r="P878" s="10"/>
@@ -36757,7 +36784,7 @@
       <c r="L879" s="30"/>
       <c r="M879" s="80"/>
       <c r="N879" s="37"/>
-      <c r="O879" s="176">
+      <c r="O879" s="174">
         <v>221</v>
       </c>
       <c r="P879" s="10"/>
@@ -36798,7 +36825,7 @@
       <c r="L880" s="30"/>
       <c r="M880" s="80"/>
       <c r="N880" s="37"/>
-      <c r="O880" s="176">
+      <c r="O880" s="174">
         <v>213</v>
       </c>
       <c r="P880" s="10"/>
@@ -36835,8 +36862,8 @@
       <c r="L881" s="10"/>
       <c r="M881" s="40"/>
       <c r="N881" s="37"/>
-      <c r="O881" s="176" t="s">
-        <v>227</v>
+      <c r="O881" s="174" t="s">
+        <v>226</v>
       </c>
       <c r="P881" s="10"/>
       <c r="Q881" s="44" t="s">
@@ -36874,7 +36901,7 @@
       <c r="L882" s="10"/>
       <c r="M882" s="40"/>
       <c r="N882" s="37"/>
-      <c r="O882" s="176"/>
+      <c r="O882" s="174"/>
       <c r="P882" s="10"/>
       <c r="Q882" s="44" t="s">
         <v>15</v>
@@ -36911,8 +36938,8 @@
       <c r="L883" s="10"/>
       <c r="M883" s="40"/>
       <c r="N883" s="37"/>
-      <c r="O883" s="176" t="s">
-        <v>228</v>
+      <c r="O883" s="174" t="s">
+        <v>227</v>
       </c>
       <c r="P883" s="10"/>
       <c r="Q883" s="44" t="s">
@@ -36950,7 +36977,7 @@
       <c r="L884" s="10"/>
       <c r="M884" s="40"/>
       <c r="N884" s="37"/>
-      <c r="O884" s="176" t="s">
+      <c r="O884" s="174" t="s">
         <v>23</v>
       </c>
       <c r="P884" s="10"/>
@@ -36989,7 +37016,7 @@
       <c r="L885" s="10"/>
       <c r="M885" s="40"/>
       <c r="N885" s="37"/>
-      <c r="O885" s="176" t="s">
+      <c r="O885" s="174" t="s">
         <v>28</v>
       </c>
       <c r="P885" s="10"/>
@@ -37028,7 +37055,7 @@
       <c r="L886" s="10"/>
       <c r="M886" s="40"/>
       <c r="N886" s="37"/>
-      <c r="O886" s="176" t="s">
+      <c r="O886" s="174" t="s">
         <v>31</v>
       </c>
       <c r="P886" s="10"/>
@@ -37067,8 +37094,8 @@
       <c r="L887" s="52"/>
       <c r="M887" s="54"/>
       <c r="N887" s="55"/>
-      <c r="O887" s="177" t="s">
-        <v>229</v>
+      <c r="O887" s="175" t="s">
+        <v>228</v>
       </c>
       <c r="P887" s="52"/>
       <c r="Q887" s="57" t="s">
@@ -37220,7 +37247,7 @@
       <c r="L891" s="30"/>
       <c r="M891" s="80"/>
       <c r="N891" s="37"/>
-      <c r="O891" s="226">
+      <c r="O891" s="224">
         <v>92</v>
       </c>
       <c r="P891" s="10"/>
@@ -37261,7 +37288,7 @@
       <c r="L892" s="30"/>
       <c r="M892" s="80"/>
       <c r="N892" s="37"/>
-      <c r="O892" s="226">
+      <c r="O892" s="224">
         <v>146</v>
       </c>
       <c r="P892" s="10"/>
@@ -37302,7 +37329,7 @@
       <c r="L893" s="30"/>
       <c r="M893" s="80"/>
       <c r="N893" s="37"/>
-      <c r="O893" s="226">
+      <c r="O893" s="224">
         <v>68</v>
       </c>
       <c r="P893" s="10"/>
@@ -37339,8 +37366,8 @@
       <c r="L894" s="10"/>
       <c r="M894" s="40"/>
       <c r="N894" s="37"/>
-      <c r="O894" s="226" t="s">
-        <v>230</v>
+      <c r="O894" s="224" t="s">
+        <v>229</v>
       </c>
       <c r="P894" s="10"/>
       <c r="Q894" s="44" t="s">
@@ -37378,8 +37405,8 @@
       <c r="L895" s="10"/>
       <c r="M895" s="40"/>
       <c r="N895" s="37"/>
-      <c r="O895" s="226" t="s">
-        <v>231</v>
+      <c r="O895" s="224" t="s">
+        <v>230</v>
       </c>
       <c r="P895" s="10"/>
       <c r="Q895" s="44" t="s">
@@ -37417,8 +37444,8 @@
       <c r="L896" s="10"/>
       <c r="M896" s="40"/>
       <c r="N896" s="37"/>
-      <c r="O896" s="226" t="s">
-        <v>232</v>
+      <c r="O896" s="224" t="s">
+        <v>231</v>
       </c>
       <c r="P896" s="10"/>
       <c r="Q896" s="44" t="s">
@@ -37456,7 +37483,7 @@
       <c r="L897" s="10"/>
       <c r="M897" s="40"/>
       <c r="N897" s="37"/>
-      <c r="O897" s="226" t="s">
+      <c r="O897" s="224" t="s">
         <v>23</v>
       </c>
       <c r="P897" s="10"/>
@@ -37495,7 +37522,7 @@
       <c r="L898" s="10"/>
       <c r="M898" s="40"/>
       <c r="N898" s="37"/>
-      <c r="O898" s="226" t="s">
+      <c r="O898" s="224" t="s">
         <v>28</v>
       </c>
       <c r="P898" s="10"/>
@@ -37534,7 +37561,7 @@
       <c r="L899" s="10"/>
       <c r="M899" s="40"/>
       <c r="N899" s="37"/>
-      <c r="O899" s="226" t="s">
+      <c r="O899" s="224" t="s">
         <v>31</v>
       </c>
       <c r="P899" s="10"/>
@@ -37573,8 +37600,8 @@
       <c r="L900" s="52"/>
       <c r="M900" s="54"/>
       <c r="N900" s="55"/>
-      <c r="O900" s="227" t="s">
-        <v>233</v>
+      <c r="O900" s="225" t="s">
+        <v>232</v>
       </c>
       <c r="P900" s="52"/>
       <c r="Q900" s="57" t="s">
@@ -37726,7 +37753,7 @@
       <c r="L904" s="30"/>
       <c r="M904" s="80"/>
       <c r="N904" s="37"/>
-      <c r="O904" s="228">
+      <c r="O904" s="226">
         <v>31</v>
       </c>
       <c r="P904" s="10"/>
@@ -37767,7 +37794,7 @@
       <c r="L905" s="30"/>
       <c r="M905" s="80"/>
       <c r="N905" s="37"/>
-      <c r="O905" s="228">
+      <c r="O905" s="226">
         <v>93</v>
       </c>
       <c r="P905" s="10"/>
@@ -37808,7 +37835,7 @@
       <c r="L906" s="30"/>
       <c r="M906" s="80"/>
       <c r="N906" s="37"/>
-      <c r="O906" s="228">
+      <c r="O906" s="226">
         <v>51</v>
       </c>
       <c r="P906" s="10"/>
@@ -37845,8 +37872,8 @@
       <c r="L907" s="10"/>
       <c r="M907" s="40"/>
       <c r="N907" s="37"/>
-      <c r="O907" s="228" t="s">
-        <v>234</v>
+      <c r="O907" s="226" t="s">
+        <v>233</v>
       </c>
       <c r="P907" s="10"/>
       <c r="Q907" s="44" t="s">
@@ -37884,8 +37911,8 @@
       <c r="L908" s="10"/>
       <c r="M908" s="40"/>
       <c r="N908" s="37"/>
-      <c r="O908" s="228" t="s">
-        <v>235</v>
+      <c r="O908" s="226" t="s">
+        <v>234</v>
       </c>
       <c r="P908" s="10"/>
       <c r="Q908" s="44" t="s">
@@ -37923,8 +37950,8 @@
       <c r="L909" s="10"/>
       <c r="M909" s="40"/>
       <c r="N909" s="37"/>
-      <c r="O909" s="228" t="s">
-        <v>236</v>
+      <c r="O909" s="226" t="s">
+        <v>235</v>
       </c>
       <c r="P909" s="10"/>
       <c r="Q909" s="44" t="s">
@@ -37962,7 +37989,7 @@
       <c r="L910" s="10"/>
       <c r="M910" s="40"/>
       <c r="N910" s="37"/>
-      <c r="O910" s="228" t="s">
+      <c r="O910" s="226" t="s">
         <v>23</v>
       </c>
       <c r="P910" s="10"/>
@@ -38001,7 +38028,7 @@
       <c r="L911" s="10"/>
       <c r="M911" s="40"/>
       <c r="N911" s="37"/>
-      <c r="O911" s="228" t="s">
+      <c r="O911" s="226" t="s">
         <v>117</v>
       </c>
       <c r="P911" s="10"/>
@@ -38040,8 +38067,8 @@
       <c r="L912" s="10"/>
       <c r="M912" s="40"/>
       <c r="N912" s="37"/>
-      <c r="O912" s="228" t="s">
-        <v>208</v>
+      <c r="O912" s="226" t="s">
+        <v>207</v>
       </c>
       <c r="P912" s="10"/>
       <c r="Q912" s="44" t="s">
@@ -38079,8 +38106,8 @@
       <c r="L913" s="52"/>
       <c r="M913" s="54"/>
       <c r="N913" s="55"/>
-      <c r="O913" s="229" t="s">
-        <v>237</v>
+      <c r="O913" s="227" t="s">
+        <v>236</v>
       </c>
       <c r="P913" s="52"/>
       <c r="Q913" s="57" t="s">
@@ -38232,7 +38259,7 @@
       <c r="L917" s="30"/>
       <c r="M917" s="80"/>
       <c r="N917" s="37"/>
-      <c r="O917" s="178">
+      <c r="O917" s="176">
         <v>30</v>
       </c>
       <c r="P917" s="10"/>
@@ -38273,7 +38300,7 @@
       <c r="L918" s="30"/>
       <c r="M918" s="80"/>
       <c r="N918" s="37"/>
-      <c r="O918" s="178">
+      <c r="O918" s="176">
         <v>109</v>
       </c>
       <c r="P918" s="10"/>
@@ -38314,7 +38341,7 @@
       <c r="L919" s="30"/>
       <c r="M919" s="80"/>
       <c r="N919" s="37"/>
-      <c r="O919" s="178">
+      <c r="O919" s="176">
         <v>53</v>
       </c>
       <c r="P919" s="10"/>
@@ -38351,8 +38378,8 @@
       <c r="L920" s="10"/>
       <c r="M920" s="40"/>
       <c r="N920" s="37"/>
-      <c r="O920" s="178" t="s">
-        <v>238</v>
+      <c r="O920" s="176" t="s">
+        <v>237</v>
       </c>
       <c r="P920" s="10"/>
       <c r="Q920" s="44" t="s">
@@ -38390,7 +38417,7 @@
       <c r="L921" s="10"/>
       <c r="M921" s="40"/>
       <c r="N921" s="37"/>
-      <c r="O921" s="178"/>
+      <c r="O921" s="176"/>
       <c r="P921" s="10"/>
       <c r="Q921" s="44" t="s">
         <v>15</v>
@@ -38427,8 +38454,8 @@
       <c r="L922" s="10"/>
       <c r="M922" s="40"/>
       <c r="N922" s="37"/>
-      <c r="O922" s="178" t="s">
-        <v>239</v>
+      <c r="O922" s="176" t="s">
+        <v>238</v>
       </c>
       <c r="P922" s="10"/>
       <c r="Q922" s="44" t="s">
@@ -38466,7 +38493,7 @@
       <c r="L923" s="10"/>
       <c r="M923" s="40"/>
       <c r="N923" s="37"/>
-      <c r="O923" s="178" t="s">
+      <c r="O923" s="176" t="s">
         <v>23</v>
       </c>
       <c r="P923" s="10"/>
@@ -38505,8 +38532,8 @@
       <c r="L924" s="10"/>
       <c r="M924" s="40"/>
       <c r="N924" s="37"/>
-      <c r="O924" s="178" t="s">
-        <v>206</v>
+      <c r="O924" s="176" t="s">
+        <v>205</v>
       </c>
       <c r="P924" s="10"/>
       <c r="Q924" s="44" t="s">
@@ -38544,8 +38571,8 @@
       <c r="L925" s="10"/>
       <c r="M925" s="40"/>
       <c r="N925" s="37"/>
-      <c r="O925" s="178" t="s">
-        <v>208</v>
+      <c r="O925" s="176" t="s">
+        <v>207</v>
       </c>
       <c r="P925" s="10"/>
       <c r="Q925" s="44" t="s">
@@ -38583,8 +38610,8 @@
       <c r="L926" s="52"/>
       <c r="M926" s="54"/>
       <c r="N926" s="55"/>
-      <c r="O926" s="179" t="s">
-        <v>240</v>
+      <c r="O926" s="177" t="s">
+        <v>239</v>
       </c>
       <c r="P926" s="52"/>
       <c r="Q926" s="57" t="s">
@@ -38736,7 +38763,7 @@
       <c r="L930" s="30"/>
       <c r="M930" s="80"/>
       <c r="N930" s="37"/>
-      <c r="O930" s="180">
+      <c r="O930" s="178">
         <v>58</v>
       </c>
       <c r="P930" s="10"/>
@@ -38777,7 +38804,7 @@
       <c r="L931" s="30"/>
       <c r="M931" s="80"/>
       <c r="N931" s="37"/>
-      <c r="O931" s="180">
+      <c r="O931" s="178">
         <v>91</v>
       </c>
       <c r="P931" s="10"/>
@@ -38818,7 +38845,7 @@
       <c r="L932" s="30"/>
       <c r="M932" s="80"/>
       <c r="N932" s="37"/>
-      <c r="O932" s="180">
+      <c r="O932" s="178">
         <v>54</v>
       </c>
       <c r="P932" s="10"/>
@@ -38855,8 +38882,8 @@
       <c r="L933" s="10"/>
       <c r="M933" s="40"/>
       <c r="N933" s="37"/>
-      <c r="O933" s="180" t="s">
-        <v>241</v>
+      <c r="O933" s="178" t="s">
+        <v>240</v>
       </c>
       <c r="P933" s="10"/>
       <c r="Q933" s="44" t="s">
@@ -38894,7 +38921,7 @@
       <c r="L934" s="10"/>
       <c r="M934" s="40"/>
       <c r="N934" s="37"/>
-      <c r="O934" s="180"/>
+      <c r="O934" s="178"/>
       <c r="P934" s="10"/>
       <c r="Q934" s="44" t="s">
         <v>15</v>
@@ -38931,8 +38958,8 @@
       <c r="L935" s="10"/>
       <c r="M935" s="40"/>
       <c r="N935" s="37"/>
-      <c r="O935" s="180" t="s">
-        <v>243</v>
+      <c r="O935" s="178" t="s">
+        <v>242</v>
       </c>
       <c r="P935" s="10"/>
       <c r="Q935" s="44" t="s">
@@ -38970,7 +38997,7 @@
       <c r="L936" s="10"/>
       <c r="M936" s="40"/>
       <c r="N936" s="37"/>
-      <c r="O936" s="180" t="s">
+      <c r="O936" s="178" t="s">
         <v>23</v>
       </c>
       <c r="P936" s="10"/>
@@ -39009,8 +39036,8 @@
       <c r="L937" s="10"/>
       <c r="M937" s="40"/>
       <c r="N937" s="37"/>
-      <c r="O937" s="180" t="s">
-        <v>242</v>
+      <c r="O937" s="178" t="s">
+        <v>241</v>
       </c>
       <c r="P937" s="10"/>
       <c r="Q937" s="44" t="s">
@@ -39048,8 +39075,8 @@
       <c r="L938" s="10"/>
       <c r="M938" s="40"/>
       <c r="N938" s="37"/>
-      <c r="O938" s="180" t="s">
-        <v>211</v>
+      <c r="O938" s="178" t="s">
+        <v>210</v>
       </c>
       <c r="P938" s="10"/>
       <c r="Q938" s="44" t="s">
@@ -39087,8 +39114,8 @@
       <c r="L939" s="52"/>
       <c r="M939" s="54"/>
       <c r="N939" s="55"/>
-      <c r="O939" s="181" t="s">
-        <v>244</v>
+      <c r="O939" s="179" t="s">
+        <v>243</v>
       </c>
       <c r="P939" s="52"/>
       <c r="Q939" s="57" t="s">
@@ -39240,7 +39267,7 @@
       <c r="L943" s="30"/>
       <c r="M943" s="80"/>
       <c r="N943" s="37"/>
-      <c r="O943" s="182">
+      <c r="O943" s="180">
         <v>25</v>
       </c>
       <c r="P943" s="10"/>
@@ -39281,7 +39308,7 @@
       <c r="L944" s="30"/>
       <c r="M944" s="80"/>
       <c r="N944" s="37"/>
-      <c r="O944" s="182">
+      <c r="O944" s="180">
         <v>89</v>
       </c>
       <c r="P944" s="10"/>
@@ -39322,7 +39349,7 @@
       <c r="L945" s="30"/>
       <c r="M945" s="80"/>
       <c r="N945" s="37"/>
-      <c r="O945" s="182">
+      <c r="O945" s="180">
         <v>99</v>
       </c>
       <c r="P945" s="10"/>
@@ -39359,8 +39386,8 @@
       <c r="L946" s="10"/>
       <c r="M946" s="40"/>
       <c r="N946" s="37"/>
-      <c r="O946" s="182" t="s">
-        <v>245</v>
+      <c r="O946" s="180" t="s">
+        <v>244</v>
       </c>
       <c r="P946" s="10"/>
       <c r="Q946" s="44" t="s">
@@ -39398,7 +39425,7 @@
       <c r="L947" s="10"/>
       <c r="M947" s="40"/>
       <c r="N947" s="37"/>
-      <c r="O947" s="182"/>
+      <c r="O947" s="180"/>
       <c r="P947" s="10"/>
       <c r="Q947" s="44" t="s">
         <v>15</v>
@@ -39435,8 +39462,8 @@
       <c r="L948" s="10"/>
       <c r="M948" s="40"/>
       <c r="N948" s="37"/>
-      <c r="O948" s="182" t="s">
-        <v>248</v>
+      <c r="O948" s="180" t="s">
+        <v>247</v>
       </c>
       <c r="P948" s="10"/>
       <c r="Q948" s="44" t="s">
@@ -39474,7 +39501,7 @@
       <c r="L949" s="10"/>
       <c r="M949" s="40"/>
       <c r="N949" s="37"/>
-      <c r="O949" s="182" t="s">
+      <c r="O949" s="180" t="s">
         <v>23</v>
       </c>
       <c r="P949" s="10"/>
@@ -39513,8 +39540,8 @@
       <c r="L950" s="10"/>
       <c r="M950" s="40"/>
       <c r="N950" s="37"/>
-      <c r="O950" s="182" t="s">
-        <v>246</v>
+      <c r="O950" s="180" t="s">
+        <v>245</v>
       </c>
       <c r="P950" s="10"/>
       <c r="Q950" s="44" t="s">
@@ -39552,8 +39579,8 @@
       <c r="L951" s="10"/>
       <c r="M951" s="40"/>
       <c r="N951" s="37"/>
-      <c r="O951" s="182" t="s">
-        <v>208</v>
+      <c r="O951" s="180" t="s">
+        <v>207</v>
       </c>
       <c r="P951" s="10"/>
       <c r="Q951" s="44" t="s">
@@ -39591,8 +39618,8 @@
       <c r="L952" s="52"/>
       <c r="M952" s="54"/>
       <c r="N952" s="55"/>
-      <c r="O952" s="183" t="s">
-        <v>247</v>
+      <c r="O952" s="181" t="s">
+        <v>246</v>
       </c>
       <c r="P952" s="52"/>
       <c r="Q952" s="57" t="s">
@@ -39744,7 +39771,7 @@
       <c r="L956" s="30"/>
       <c r="M956" s="80"/>
       <c r="N956" s="37"/>
-      <c r="O956" s="184">
+      <c r="O956" s="182">
         <v>174</v>
       </c>
       <c r="P956" s="10"/>
@@ -39785,7 +39812,7 @@
       <c r="L957" s="30"/>
       <c r="M957" s="80"/>
       <c r="N957" s="37"/>
-      <c r="O957" s="184">
+      <c r="O957" s="182">
         <v>121</v>
       </c>
       <c r="P957" s="10"/>
@@ -39826,7 +39853,7 @@
       <c r="L958" s="30"/>
       <c r="M958" s="80"/>
       <c r="N958" s="37"/>
-      <c r="O958" s="184">
+      <c r="O958" s="182">
         <v>72</v>
       </c>
       <c r="P958" s="10"/>
@@ -39863,8 +39890,8 @@
       <c r="L959" s="10"/>
       <c r="M959" s="40"/>
       <c r="N959" s="37"/>
-      <c r="O959" s="184" t="s">
-        <v>249</v>
+      <c r="O959" s="182" t="s">
+        <v>248</v>
       </c>
       <c r="P959" s="10"/>
       <c r="Q959" s="44" t="s">
@@ -39902,7 +39929,7 @@
       <c r="L960" s="10"/>
       <c r="M960" s="40"/>
       <c r="N960" s="37"/>
-      <c r="O960" s="184"/>
+      <c r="O960" s="182"/>
       <c r="P960" s="10"/>
       <c r="Q960" s="44" t="s">
         <v>15</v>
@@ -39939,8 +39966,8 @@
       <c r="L961" s="10"/>
       <c r="M961" s="40"/>
       <c r="N961" s="37"/>
-      <c r="O961" s="184" t="s">
-        <v>250</v>
+      <c r="O961" s="182" t="s">
+        <v>249</v>
       </c>
       <c r="P961" s="10"/>
       <c r="Q961" s="44" t="s">
@@ -39978,7 +40005,7 @@
       <c r="L962" s="10"/>
       <c r="M962" s="40"/>
       <c r="N962" s="37"/>
-      <c r="O962" s="184" t="s">
+      <c r="O962" s="182" t="s">
         <v>23</v>
       </c>
       <c r="P962" s="10"/>
@@ -40017,8 +40044,8 @@
       <c r="L963" s="10"/>
       <c r="M963" s="40"/>
       <c r="N963" s="37"/>
-      <c r="O963" s="184" t="s">
-        <v>246</v>
+      <c r="O963" s="182" t="s">
+        <v>245</v>
       </c>
       <c r="P963" s="10"/>
       <c r="Q963" s="44" t="s">
@@ -40056,8 +40083,8 @@
       <c r="L964" s="10"/>
       <c r="M964" s="40"/>
       <c r="N964" s="37"/>
-      <c r="O964" s="184" t="s">
-        <v>208</v>
+      <c r="O964" s="182" t="s">
+        <v>207</v>
       </c>
       <c r="P964" s="10"/>
       <c r="Q964" s="44" t="s">
@@ -40095,8 +40122,8 @@
       <c r="L965" s="52"/>
       <c r="M965" s="54"/>
       <c r="N965" s="55"/>
-      <c r="O965" s="185" t="s">
-        <v>251</v>
+      <c r="O965" s="183" t="s">
+        <v>250</v>
       </c>
       <c r="P965" s="52"/>
       <c r="Q965" s="57" t="s">
@@ -40248,7 +40275,7 @@
       <c r="L969" s="30"/>
       <c r="M969" s="80"/>
       <c r="N969" s="37"/>
-      <c r="O969" s="186">
+      <c r="O969" s="184">
         <v>28</v>
       </c>
       <c r="P969" s="10"/>
@@ -40289,7 +40316,7 @@
       <c r="L970" s="30"/>
       <c r="M970" s="80"/>
       <c r="N970" s="37"/>
-      <c r="O970" s="186">
+      <c r="O970" s="184">
         <v>48</v>
       </c>
       <c r="P970" s="10"/>
@@ -40330,7 +40357,7 @@
       <c r="L971" s="30"/>
       <c r="M971" s="80"/>
       <c r="N971" s="37"/>
-      <c r="O971" s="186">
+      <c r="O971" s="184">
         <v>173</v>
       </c>
       <c r="P971" s="10"/>
@@ -40367,8 +40394,8 @@
       <c r="L972" s="10"/>
       <c r="M972" s="40"/>
       <c r="N972" s="37"/>
-      <c r="O972" s="186" t="s">
-        <v>252</v>
+      <c r="O972" s="184" t="s">
+        <v>251</v>
       </c>
       <c r="P972" s="10"/>
       <c r="Q972" s="44" t="s">
@@ -40406,8 +40433,8 @@
       <c r="L973" s="10"/>
       <c r="M973" s="40"/>
       <c r="N973" s="37"/>
-      <c r="O973" s="186" t="s">
-        <v>253</v>
+      <c r="O973" s="184" t="s">
+        <v>252</v>
       </c>
       <c r="P973" s="10"/>
       <c r="Q973" s="44" t="s">
@@ -40445,8 +40472,8 @@
       <c r="L974" s="10"/>
       <c r="M974" s="40"/>
       <c r="N974" s="37"/>
-      <c r="O974" s="186" t="s">
-        <v>254</v>
+      <c r="O974" s="184" t="s">
+        <v>253</v>
       </c>
       <c r="P974" s="10"/>
       <c r="Q974" s="44" t="s">
@@ -40484,7 +40511,7 @@
       <c r="L975" s="10"/>
       <c r="M975" s="40"/>
       <c r="N975" s="37"/>
-      <c r="O975" s="186" t="s">
+      <c r="O975" s="184" t="s">
         <v>23</v>
       </c>
       <c r="P975" s="10"/>
@@ -40523,7 +40550,7 @@
       <c r="L976" s="10"/>
       <c r="M976" s="40"/>
       <c r="N976" s="37"/>
-      <c r="O976" s="186" t="s">
+      <c r="O976" s="184" t="s">
         <v>117</v>
       </c>
       <c r="P976" s="10"/>
@@ -40562,8 +40589,8 @@
       <c r="L977" s="10"/>
       <c r="M977" s="40"/>
       <c r="N977" s="37"/>
-      <c r="O977" s="186" t="s">
-        <v>208</v>
+      <c r="O977" s="184" t="s">
+        <v>207</v>
       </c>
       <c r="P977" s="10"/>
       <c r="Q977" s="44" t="s">
@@ -40601,8 +40628,8 @@
       <c r="L978" s="52"/>
       <c r="M978" s="54"/>
       <c r="N978" s="55"/>
-      <c r="O978" s="187" t="s">
-        <v>255</v>
+      <c r="O978" s="185" t="s">
+        <v>254</v>
       </c>
       <c r="P978" s="52"/>
       <c r="Q978" s="57" t="s">
@@ -40754,7 +40781,7 @@
       <c r="L982" s="30"/>
       <c r="M982" s="80"/>
       <c r="N982" s="37"/>
-      <c r="O982" s="188">
+      <c r="O982" s="186">
         <v>254</v>
       </c>
       <c r="P982" s="10"/>
@@ -40795,7 +40822,7 @@
       <c r="L983" s="30"/>
       <c r="M983" s="80"/>
       <c r="N983" s="37"/>
-      <c r="O983" s="188">
+      <c r="O983" s="186">
         <v>241</v>
       </c>
       <c r="P983" s="10"/>
@@ -40836,7 +40863,7 @@
       <c r="L984" s="30"/>
       <c r="M984" s="80"/>
       <c r="N984" s="37"/>
-      <c r="O984" s="188">
+      <c r="O984" s="186">
         <v>213</v>
       </c>
       <c r="P984" s="10"/>
@@ -40873,8 +40900,8 @@
       <c r="L985" s="10"/>
       <c r="M985" s="40"/>
       <c r="N985" s="37"/>
-      <c r="O985" s="188" t="s">
-        <v>256</v>
+      <c r="O985" s="186" t="s">
+        <v>255</v>
       </c>
       <c r="P985" s="10"/>
       <c r="Q985" s="44" t="s">
@@ -40912,8 +40939,8 @@
       <c r="L986" s="10"/>
       <c r="M986" s="40"/>
       <c r="N986" s="37"/>
-      <c r="O986" s="188" t="s">
-        <v>257</v>
+      <c r="O986" s="186" t="s">
+        <v>256</v>
       </c>
       <c r="P986" s="10"/>
       <c r="Q986" s="44" t="s">
@@ -40951,8 +40978,8 @@
       <c r="L987" s="10"/>
       <c r="M987" s="40"/>
       <c r="N987" s="37"/>
-      <c r="O987" s="188" t="s">
-        <v>258</v>
+      <c r="O987" s="186" t="s">
+        <v>257</v>
       </c>
       <c r="P987" s="10"/>
       <c r="Q987" s="44" t="s">
@@ -40990,7 +41017,7 @@
       <c r="L988" s="10"/>
       <c r="M988" s="40"/>
       <c r="N988" s="37"/>
-      <c r="O988" s="188" t="s">
+      <c r="O988" s="186" t="s">
         <v>23</v>
       </c>
       <c r="P988" s="10"/>
@@ -41029,7 +41056,7 @@
       <c r="L989" s="10"/>
       <c r="M989" s="40"/>
       <c r="N989" s="37"/>
-      <c r="O989" s="188" t="s">
+      <c r="O989" s="186" t="s">
         <v>28</v>
       </c>
       <c r="P989" s="10"/>
@@ -41068,7 +41095,7 @@
       <c r="L990" s="10"/>
       <c r="M990" s="40"/>
       <c r="N990" s="37"/>
-      <c r="O990" s="188" t="s">
+      <c r="O990" s="186" t="s">
         <v>31</v>
       </c>
       <c r="P990" s="10"/>
@@ -41107,8 +41134,8 @@
       <c r="L991" s="52"/>
       <c r="M991" s="54"/>
       <c r="N991" s="55"/>
-      <c r="O991" s="189" t="s">
-        <v>259</v>
+      <c r="O991" s="187" t="s">
+        <v>258</v>
       </c>
       <c r="P991" s="52"/>
       <c r="Q991" s="57" t="s">
@@ -41260,7 +41287,7 @@
       <c r="L995" s="30"/>
       <c r="M995" s="80"/>
       <c r="N995" s="37"/>
-      <c r="O995" s="190">
+      <c r="O995" s="188">
         <v>255</v>
       </c>
       <c r="P995" s="10"/>
@@ -41301,7 +41328,7 @@
       <c r="L996" s="30"/>
       <c r="M996" s="80"/>
       <c r="N996" s="37"/>
-      <c r="O996" s="190">
+      <c r="O996" s="188">
         <v>249</v>
       </c>
       <c r="P996" s="10"/>
@@ -41342,7 +41369,7 @@
       <c r="L997" s="30"/>
       <c r="M997" s="80"/>
       <c r="N997" s="37"/>
-      <c r="O997" s="190">
+      <c r="O997" s="188">
         <v>106</v>
       </c>
       <c r="P997" s="10"/>
@@ -41379,8 +41406,8 @@
       <c r="L998" s="10"/>
       <c r="M998" s="40"/>
       <c r="N998" s="37"/>
-      <c r="O998" s="190" t="s">
-        <v>260</v>
+      <c r="O998" s="188" t="s">
+        <v>259</v>
       </c>
       <c r="P998" s="10"/>
       <c r="Q998" s="44" t="s">
@@ -41418,8 +41445,8 @@
       <c r="L999" s="10"/>
       <c r="M999" s="40"/>
       <c r="N999" s="37"/>
-      <c r="O999" s="190" t="s">
-        <v>261</v>
+      <c r="O999" s="188" t="s">
+        <v>260</v>
       </c>
       <c r="P999" s="10"/>
       <c r="Q999" s="44" t="s">
@@ -41457,8 +41484,8 @@
       <c r="L1000" s="10"/>
       <c r="M1000" s="40"/>
       <c r="N1000" s="37"/>
-      <c r="O1000" s="190" t="s">
-        <v>262</v>
+      <c r="O1000" s="188" t="s">
+        <v>261</v>
       </c>
       <c r="P1000" s="10"/>
       <c r="Q1000" s="44" t="s">
@@ -41496,7 +41523,7 @@
       <c r="L1001" s="10"/>
       <c r="M1001" s="40"/>
       <c r="N1001" s="37"/>
-      <c r="O1001" s="190" t="s">
+      <c r="O1001" s="188" t="s">
         <v>23</v>
       </c>
       <c r="P1001" s="10"/>
@@ -41535,7 +41562,7 @@
       <c r="L1002" s="10"/>
       <c r="M1002" s="40"/>
       <c r="N1002" s="37"/>
-      <c r="O1002" s="190" t="s">
+      <c r="O1002" s="188" t="s">
         <v>28</v>
       </c>
       <c r="P1002" s="10"/>
@@ -41574,7 +41601,7 @@
       <c r="L1003" s="10"/>
       <c r="M1003" s="40"/>
       <c r="N1003" s="37"/>
-      <c r="O1003" s="190" t="s">
+      <c r="O1003" s="188" t="s">
         <v>31</v>
       </c>
       <c r="P1003" s="10"/>
@@ -41613,8 +41640,8 @@
       <c r="L1004" s="52"/>
       <c r="M1004" s="54"/>
       <c r="N1004" s="55"/>
-      <c r="O1004" s="191" t="s">
-        <v>263</v>
+      <c r="O1004" s="189" t="s">
+        <v>262</v>
       </c>
       <c r="P1004" s="52"/>
       <c r="Q1004" s="57" t="s">
@@ -41766,7 +41793,7 @@
       <c r="L1008" s="30"/>
       <c r="M1008" s="80"/>
       <c r="N1008" s="37"/>
-      <c r="O1008" s="192">
+      <c r="O1008" s="190">
         <v>255</v>
       </c>
       <c r="P1008" s="10"/>
@@ -41807,7 +41834,7 @@
       <c r="L1009" s="30"/>
       <c r="M1009" s="80"/>
       <c r="N1009" s="37"/>
-      <c r="O1009" s="192">
+      <c r="O1009" s="190">
         <v>238</v>
       </c>
       <c r="P1009" s="10"/>
@@ -41848,7 +41875,7 @@
       <c r="L1010" s="30"/>
       <c r="M1010" s="80"/>
       <c r="N1010" s="37"/>
-      <c r="O1010" s="192">
+      <c r="O1010" s="190">
         <v>32</v>
       </c>
       <c r="P1010" s="10"/>
@@ -41885,8 +41912,8 @@
       <c r="L1011" s="10"/>
       <c r="M1011" s="40"/>
       <c r="N1011" s="37"/>
-      <c r="O1011" s="192" t="s">
-        <v>264</v>
+      <c r="O1011" s="190" t="s">
+        <v>263</v>
       </c>
       <c r="P1011" s="10"/>
       <c r="Q1011" s="44" t="s">
@@ -41924,8 +41951,8 @@
       <c r="L1012" s="10"/>
       <c r="M1012" s="40"/>
       <c r="N1012" s="37"/>
-      <c r="O1012" s="192" t="s">
-        <v>265</v>
+      <c r="O1012" s="190" t="s">
+        <v>264</v>
       </c>
       <c r="P1012" s="10"/>
       <c r="Q1012" s="44" t="s">
@@ -41963,8 +41990,8 @@
       <c r="L1013" s="10"/>
       <c r="M1013" s="40"/>
       <c r="N1013" s="37"/>
-      <c r="O1013" s="192" t="s">
-        <v>266</v>
+      <c r="O1013" s="190" t="s">
+        <v>265</v>
       </c>
       <c r="P1013" s="10"/>
       <c r="Q1013" s="44" t="s">
@@ -42002,7 +42029,7 @@
       <c r="L1014" s="10"/>
       <c r="M1014" s="40"/>
       <c r="N1014" s="37"/>
-      <c r="O1014" s="192" t="s">
+      <c r="O1014" s="190" t="s">
         <v>23</v>
       </c>
       <c r="P1014" s="10"/>
@@ -42041,7 +42068,7 @@
       <c r="L1015" s="10"/>
       <c r="M1015" s="40"/>
       <c r="N1015" s="37"/>
-      <c r="O1015" s="192" t="s">
+      <c r="O1015" s="190" t="s">
         <v>28</v>
       </c>
       <c r="P1015" s="10"/>
@@ -42080,7 +42107,7 @@
       <c r="L1016" s="10"/>
       <c r="M1016" s="40"/>
       <c r="N1016" s="37"/>
-      <c r="O1016" s="192" t="s">
+      <c r="O1016" s="190" t="s">
         <v>31</v>
       </c>
       <c r="P1016" s="10"/>
@@ -42119,8 +42146,8 @@
       <c r="L1017" s="52"/>
       <c r="M1017" s="54"/>
       <c r="N1017" s="55"/>
-      <c r="O1017" s="193" t="s">
-        <v>267</v>
+      <c r="O1017" s="191" t="s">
+        <v>266</v>
       </c>
       <c r="P1017" s="52"/>
       <c r="Q1017" s="57" t="s">
@@ -42272,7 +42299,7 @@
       <c r="L1021" s="30"/>
       <c r="M1021" s="80"/>
       <c r="N1021" s="37"/>
-      <c r="O1021" s="194">
+      <c r="O1021" s="192">
         <v>255</v>
       </c>
       <c r="P1021" s="10"/>
@@ -42313,7 +42340,7 @@
       <c r="L1022" s="30"/>
       <c r="M1022" s="80"/>
       <c r="N1022" s="37"/>
-      <c r="O1022" s="194">
+      <c r="O1022" s="192">
         <v>211</v>
       </c>
       <c r="P1022" s="10"/>
@@ -42354,7 +42381,7 @@
       <c r="L1023" s="30"/>
       <c r="M1023" s="80"/>
       <c r="N1023" s="37"/>
-      <c r="O1023" s="194">
+      <c r="O1023" s="192">
         <v>6</v>
       </c>
       <c r="P1023" s="10"/>
@@ -42391,8 +42418,8 @@
       <c r="L1024" s="10"/>
       <c r="M1024" s="40"/>
       <c r="N1024" s="37"/>
-      <c r="O1024" s="194" t="s">
-        <v>268</v>
+      <c r="O1024" s="192" t="s">
+        <v>267</v>
       </c>
       <c r="P1024" s="10"/>
       <c r="Q1024" s="44" t="s">
@@ -42430,8 +42457,8 @@
       <c r="L1025" s="10"/>
       <c r="M1025" s="40"/>
       <c r="N1025" s="37"/>
-      <c r="O1025" s="194" t="s">
-        <v>269</v>
+      <c r="O1025" s="192" t="s">
+        <v>268</v>
       </c>
       <c r="P1025" s="10"/>
       <c r="Q1025" s="44" t="s">
@@ -42469,8 +42496,8 @@
       <c r="L1026" s="10"/>
       <c r="M1026" s="40"/>
       <c r="N1026" s="37"/>
-      <c r="O1026" s="194" t="s">
-        <v>270</v>
+      <c r="O1026" s="192" t="s">
+        <v>269</v>
       </c>
       <c r="P1026" s="10"/>
       <c r="Q1026" s="44" t="s">
@@ -42508,7 +42535,7 @@
       <c r="L1027" s="10"/>
       <c r="M1027" s="40"/>
       <c r="N1027" s="37"/>
-      <c r="O1027" s="194" t="s">
+      <c r="O1027" s="192" t="s">
         <v>23</v>
       </c>
       <c r="P1027" s="10"/>
@@ -42547,7 +42574,7 @@
       <c r="L1028" s="10"/>
       <c r="M1028" s="40"/>
       <c r="N1028" s="37"/>
-      <c r="O1028" s="194" t="s">
+      <c r="O1028" s="192" t="s">
         <v>28</v>
       </c>
       <c r="P1028" s="10"/>
@@ -42586,7 +42613,7 @@
       <c r="L1029" s="10"/>
       <c r="M1029" s="40"/>
       <c r="N1029" s="37"/>
-      <c r="O1029" s="194" t="s">
+      <c r="O1029" s="192" t="s">
         <v>31</v>
       </c>
       <c r="P1029" s="10"/>
@@ -42625,8 +42652,8 @@
       <c r="L1030" s="52"/>
       <c r="M1030" s="54"/>
       <c r="N1030" s="55"/>
-      <c r="O1030" s="195" t="s">
-        <v>271</v>
+      <c r="O1030" s="193" t="s">
+        <v>270</v>
       </c>
       <c r="P1030" s="52"/>
       <c r="Q1030" s="57" t="s">
@@ -42778,7 +42805,7 @@
       <c r="L1034" s="30"/>
       <c r="M1034" s="80"/>
       <c r="N1034" s="37"/>
-      <c r="O1034" s="196">
+      <c r="O1034" s="194">
         <v>165</v>
       </c>
       <c r="P1034" s="10"/>
@@ -42819,7 +42846,7 @@
       <c r="L1035" s="30"/>
       <c r="M1035" s="80"/>
       <c r="N1035" s="37"/>
-      <c r="O1035" s="196">
+      <c r="O1035" s="194">
         <v>165</v>
       </c>
       <c r="P1035" s="10"/>
@@ -42860,7 +42887,7 @@
       <c r="L1036" s="30"/>
       <c r="M1036" s="80"/>
       <c r="N1036" s="37"/>
-      <c r="O1036" s="196">
+      <c r="O1036" s="194">
         <v>86</v>
       </c>
       <c r="P1036" s="10"/>
@@ -42897,8 +42924,8 @@
       <c r="L1037" s="10"/>
       <c r="M1037" s="40"/>
       <c r="N1037" s="37"/>
-      <c r="O1037" s="196" t="s">
-        <v>272</v>
+      <c r="O1037" s="194" t="s">
+        <v>271</v>
       </c>
       <c r="P1037" s="10"/>
       <c r="Q1037" s="44" t="s">
@@ -42936,8 +42963,8 @@
       <c r="L1038" s="10"/>
       <c r="M1038" s="40"/>
       <c r="N1038" s="37"/>
-      <c r="O1038" s="196" t="s">
-        <v>273</v>
+      <c r="O1038" s="194" t="s">
+        <v>272</v>
       </c>
       <c r="P1038" s="10"/>
       <c r="Q1038" s="44" t="s">
@@ -42975,8 +43002,8 @@
       <c r="L1039" s="10"/>
       <c r="M1039" s="40"/>
       <c r="N1039" s="37"/>
-      <c r="O1039" s="196" t="s">
-        <v>274</v>
+      <c r="O1039" s="194" t="s">
+        <v>273</v>
       </c>
       <c r="P1039" s="10"/>
       <c r="Q1039" s="44" t="s">
@@ -43014,7 +43041,7 @@
       <c r="L1040" s="10"/>
       <c r="M1040" s="40"/>
       <c r="N1040" s="37"/>
-      <c r="O1040" s="196" t="s">
+      <c r="O1040" s="194" t="s">
         <v>23</v>
       </c>
       <c r="P1040" s="10"/>
@@ -43053,7 +43080,7 @@
       <c r="L1041" s="10"/>
       <c r="M1041" s="40"/>
       <c r="N1041" s="37"/>
-      <c r="O1041" s="196" t="s">
+      <c r="O1041" s="194" t="s">
         <v>28</v>
       </c>
       <c r="P1041" s="10"/>
@@ -43092,7 +43119,7 @@
       <c r="L1042" s="10"/>
       <c r="M1042" s="40"/>
       <c r="N1042" s="37"/>
-      <c r="O1042" s="196" t="s">
+      <c r="O1042" s="194" t="s">
         <v>31</v>
       </c>
       <c r="P1042" s="10"/>
@@ -43131,8 +43158,8 @@
       <c r="L1043" s="52"/>
       <c r="M1043" s="54"/>
       <c r="N1043" s="55"/>
-      <c r="O1043" s="197" t="s">
-        <v>275</v>
+      <c r="O1043" s="195" t="s">
+        <v>274</v>
       </c>
       <c r="P1043" s="52"/>
       <c r="Q1043" s="57" t="s">
@@ -43284,7 +43311,7 @@
       <c r="L1047" s="30"/>
       <c r="M1047" s="80"/>
       <c r="N1047" s="37"/>
-      <c r="O1047" s="198">
+      <c r="O1047" s="196">
         <v>244</v>
       </c>
       <c r="P1047" s="10"/>
@@ -43325,7 +43352,7 @@
       <c r="L1048" s="30"/>
       <c r="M1048" s="80"/>
       <c r="N1048" s="37"/>
-      <c r="O1048" s="198">
+      <c r="O1048" s="196">
         <v>124</v>
       </c>
       <c r="P1048" s="10"/>
@@ -43366,7 +43393,7 @@
       <c r="L1049" s="30"/>
       <c r="M1049" s="80"/>
       <c r="N1049" s="37"/>
-      <c r="O1049" s="198">
+      <c r="O1049" s="196">
         <v>23</v>
       </c>
       <c r="P1049" s="10"/>
@@ -43403,8 +43430,8 @@
       <c r="L1050" s="10"/>
       <c r="M1050" s="40"/>
       <c r="N1050" s="37"/>
-      <c r="O1050" s="198" t="s">
-        <v>276</v>
+      <c r="O1050" s="196" t="s">
+        <v>275</v>
       </c>
       <c r="P1050" s="10"/>
       <c r="Q1050" s="44" t="s">
@@ -43442,8 +43469,8 @@
       <c r="L1051" s="10"/>
       <c r="M1051" s="40"/>
       <c r="N1051" s="37"/>
-      <c r="O1051" s="198" t="s">
-        <v>277</v>
+      <c r="O1051" s="196" t="s">
+        <v>276</v>
       </c>
       <c r="P1051" s="10"/>
       <c r="Q1051" s="44" t="s">
@@ -43481,8 +43508,8 @@
       <c r="L1052" s="10"/>
       <c r="M1052" s="40"/>
       <c r="N1052" s="37"/>
-      <c r="O1052" s="198" t="s">
-        <v>278</v>
+      <c r="O1052" s="196" t="s">
+        <v>277</v>
       </c>
       <c r="P1052" s="10"/>
       <c r="Q1052" s="44" t="s">
@@ -43520,7 +43547,7 @@
       <c r="L1053" s="10"/>
       <c r="M1053" s="40"/>
       <c r="N1053" s="37"/>
-      <c r="O1053" s="198" t="s">
+      <c r="O1053" s="196" t="s">
         <v>23</v>
       </c>
       <c r="P1053" s="10"/>
@@ -43559,7 +43586,7 @@
       <c r="L1054" s="10"/>
       <c r="M1054" s="40"/>
       <c r="N1054" s="37"/>
-      <c r="O1054" s="198" t="s">
+      <c r="O1054" s="196" t="s">
         <v>28</v>
       </c>
       <c r="P1054" s="10"/>
@@ -43598,7 +43625,7 @@
       <c r="L1055" s="10"/>
       <c r="M1055" s="40"/>
       <c r="N1055" s="37"/>
-      <c r="O1055" s="198" t="s">
+      <c r="O1055" s="196" t="s">
         <v>31</v>
       </c>
       <c r="P1055" s="10"/>
@@ -43637,8 +43664,8 @@
       <c r="L1056" s="52"/>
       <c r="M1056" s="54"/>
       <c r="N1056" s="55"/>
-      <c r="O1056" s="199" t="s">
-        <v>279</v>
+      <c r="O1056" s="197" t="s">
+        <v>278</v>
       </c>
       <c r="P1056" s="52"/>
       <c r="Q1056" s="57" t="s">
@@ -43790,7 +43817,7 @@
       <c r="L1060" s="30"/>
       <c r="M1060" s="80"/>
       <c r="N1060" s="37"/>
-      <c r="O1060" s="200">
+      <c r="O1060" s="198">
         <v>229</v>
       </c>
       <c r="P1060" s="10"/>
@@ -43831,7 +43858,7 @@
       <c r="L1061" s="30"/>
       <c r="M1061" s="80"/>
       <c r="N1061" s="37"/>
-      <c r="O1061" s="200">
+      <c r="O1061" s="198">
         <v>64</v>
       </c>
       <c r="P1061" s="10"/>
@@ -43872,7 +43899,7 @@
       <c r="L1062" s="30"/>
       <c r="M1062" s="80"/>
       <c r="N1062" s="37"/>
-      <c r="O1062" s="200">
+      <c r="O1062" s="198">
         <v>47</v>
       </c>
       <c r="P1062" s="10"/>
@@ -43909,8 +43936,8 @@
       <c r="L1063" s="10"/>
       <c r="M1063" s="40"/>
       <c r="N1063" s="37"/>
-      <c r="O1063" s="200" t="s">
-        <v>280</v>
+      <c r="O1063" s="198" t="s">
+        <v>279</v>
       </c>
       <c r="P1063" s="10"/>
       <c r="Q1063" s="44" t="s">
@@ -43948,8 +43975,8 @@
       <c r="L1064" s="10"/>
       <c r="M1064" s="40"/>
       <c r="N1064" s="37"/>
-      <c r="O1064" s="200" t="s">
-        <v>281</v>
+      <c r="O1064" s="198" t="s">
+        <v>280</v>
       </c>
       <c r="P1064" s="10"/>
       <c r="Q1064" s="44" t="s">
@@ -43987,8 +44014,8 @@
       <c r="L1065" s="10"/>
       <c r="M1065" s="40"/>
       <c r="N1065" s="37"/>
-      <c r="O1065" s="200" t="s">
-        <v>282</v>
+      <c r="O1065" s="198" t="s">
+        <v>281</v>
       </c>
       <c r="P1065" s="10"/>
       <c r="Q1065" s="44" t="s">
@@ -44026,7 +44053,7 @@
       <c r="L1066" s="10"/>
       <c r="M1066" s="40"/>
       <c r="N1066" s="37"/>
-      <c r="O1066" s="200" t="s">
+      <c r="O1066" s="198" t="s">
         <v>23</v>
       </c>
       <c r="P1066" s="10"/>
@@ -44065,7 +44092,7 @@
       <c r="L1067" s="10"/>
       <c r="M1067" s="40"/>
       <c r="N1067" s="37"/>
-      <c r="O1067" s="200" t="s">
+      <c r="O1067" s="198" t="s">
         <v>28</v>
       </c>
       <c r="P1067" s="10"/>
@@ -44104,7 +44131,7 @@
       <c r="L1068" s="10"/>
       <c r="M1068" s="40"/>
       <c r="N1068" s="37"/>
-      <c r="O1068" s="200" t="s">
+      <c r="O1068" s="198" t="s">
         <v>31</v>
       </c>
       <c r="P1068" s="10"/>
@@ -44143,8 +44170,8 @@
       <c r="L1069" s="52"/>
       <c r="M1069" s="54"/>
       <c r="N1069" s="55"/>
-      <c r="O1069" s="201" t="s">
-        <v>283</v>
+      <c r="O1069" s="199" t="s">
+        <v>282</v>
       </c>
       <c r="P1069" s="52"/>
       <c r="Q1069" s="57" t="s">
@@ -44296,7 +44323,7 @@
       <c r="L1073" s="30"/>
       <c r="M1073" s="80"/>
       <c r="N1073" s="37"/>
-      <c r="O1073" s="202">
+      <c r="O1073" s="200">
         <v>252</v>
       </c>
       <c r="P1073" s="10"/>
@@ -44337,7 +44364,7 @@
       <c r="L1074" s="30"/>
       <c r="M1074" s="80"/>
       <c r="N1074" s="37"/>
-      <c r="O1074" s="202">
+      <c r="O1074" s="200">
         <v>57</v>
       </c>
       <c r="P1074" s="10"/>
@@ -44378,7 +44405,7 @@
       <c r="L1075" s="30"/>
       <c r="M1075" s="80"/>
       <c r="N1075" s="37"/>
-      <c r="O1075" s="202">
+      <c r="O1075" s="200">
         <v>24</v>
       </c>
       <c r="P1075" s="10"/>
@@ -44415,8 +44442,8 @@
       <c r="L1076" s="10"/>
       <c r="M1076" s="40"/>
       <c r="N1076" s="37"/>
-      <c r="O1076" s="202" t="s">
-        <v>284</v>
+      <c r="O1076" s="200" t="s">
+        <v>283</v>
       </c>
       <c r="P1076" s="10"/>
       <c r="Q1076" s="44" t="s">
@@ -44454,7 +44481,7 @@
       <c r="L1077" s="10"/>
       <c r="M1077" s="40"/>
       <c r="N1077" s="37"/>
-      <c r="O1077" s="202"/>
+      <c r="O1077" s="200"/>
       <c r="P1077" s="10"/>
       <c r="Q1077" s="44" t="s">
         <v>15</v>
@@ -44491,8 +44518,8 @@
       <c r="L1078" s="10"/>
       <c r="M1078" s="40"/>
       <c r="N1078" s="37"/>
-      <c r="O1078" s="202" t="s">
-        <v>285</v>
+      <c r="O1078" s="200" t="s">
+        <v>284</v>
       </c>
       <c r="P1078" s="10"/>
       <c r="Q1078" s="44" t="s">
@@ -44530,7 +44557,7 @@
       <c r="L1079" s="10"/>
       <c r="M1079" s="40"/>
       <c r="N1079" s="37"/>
-      <c r="O1079" s="202" t="s">
+      <c r="O1079" s="200" t="s">
         <v>23</v>
       </c>
       <c r="P1079" s="10"/>
@@ -44569,8 +44596,8 @@
       <c r="L1080" s="10"/>
       <c r="M1080" s="40"/>
       <c r="N1080" s="37"/>
-      <c r="O1080" s="202" t="s">
-        <v>206</v>
+      <c r="O1080" s="200" t="s">
+        <v>205</v>
       </c>
       <c r="P1080" s="10"/>
       <c r="Q1080" s="44" t="s">
@@ -44608,8 +44635,8 @@
       <c r="L1081" s="10"/>
       <c r="M1081" s="40"/>
       <c r="N1081" s="37"/>
-      <c r="O1081" s="202" t="s">
-        <v>208</v>
+      <c r="O1081" s="200" t="s">
+        <v>207</v>
       </c>
       <c r="P1081" s="10"/>
       <c r="Q1081" s="44" t="s">
@@ -44647,8 +44674,8 @@
       <c r="L1082" s="52"/>
       <c r="M1082" s="54"/>
       <c r="N1082" s="55"/>
-      <c r="O1082" s="203" t="s">
-        <v>286</v>
+      <c r="O1082" s="201" t="s">
+        <v>285</v>
       </c>
       <c r="P1082" s="52"/>
       <c r="Q1082" s="57" t="s">
@@ -44800,7 +44827,7 @@
       <c r="L1086" s="30"/>
       <c r="M1086" s="80"/>
       <c r="N1086" s="37"/>
-      <c r="O1086" s="204">
+      <c r="O1086" s="202">
         <v>199</v>
       </c>
       <c r="P1086" s="10"/>
@@ -44841,7 +44868,7 @@
       <c r="L1087" s="30"/>
       <c r="M1087" s="80"/>
       <c r="N1087" s="37"/>
-      <c r="O1087" s="204">
+      <c r="O1087" s="202">
         <v>154</v>
       </c>
       <c r="P1087" s="10"/>
@@ -44882,7 +44909,7 @@
       <c r="L1088" s="30"/>
       <c r="M1088" s="80"/>
       <c r="N1088" s="37"/>
-      <c r="O1088" s="204">
+      <c r="O1088" s="202">
         <v>103</v>
       </c>
       <c r="P1088" s="10"/>
@@ -44919,8 +44946,8 @@
       <c r="L1089" s="10"/>
       <c r="M1089" s="40"/>
       <c r="N1089" s="37"/>
-      <c r="O1089" s="204" t="s">
-        <v>287</v>
+      <c r="O1089" s="202" t="s">
+        <v>286</v>
       </c>
       <c r="P1089" s="10"/>
       <c r="Q1089" s="44" t="s">
@@ -44958,7 +44985,7 @@
       <c r="L1090" s="10"/>
       <c r="M1090" s="40"/>
       <c r="N1090" s="37"/>
-      <c r="O1090" s="204"/>
+      <c r="O1090" s="202"/>
       <c r="P1090" s="10"/>
       <c r="Q1090" s="44" t="s">
         <v>15</v>
@@ -44995,8 +45022,8 @@
       <c r="L1091" s="10"/>
       <c r="M1091" s="40"/>
       <c r="N1091" s="37"/>
-      <c r="O1091" s="204" t="s">
-        <v>288</v>
+      <c r="O1091" s="202" t="s">
+        <v>287</v>
       </c>
       <c r="P1091" s="10"/>
       <c r="Q1091" s="44" t="s">
@@ -45034,7 +45061,7 @@
       <c r="L1092" s="10"/>
       <c r="M1092" s="40"/>
       <c r="N1092" s="37"/>
-      <c r="O1092" s="204" t="s">
+      <c r="O1092" s="202" t="s">
         <v>23</v>
       </c>
       <c r="P1092" s="10"/>
@@ -45073,7 +45100,7 @@
       <c r="L1093" s="10"/>
       <c r="M1093" s="40"/>
       <c r="N1093" s="37"/>
-      <c r="O1093" s="204" t="s">
+      <c r="O1093" s="202" t="s">
         <v>28</v>
       </c>
       <c r="P1093" s="10"/>
@@ -45112,7 +45139,7 @@
       <c r="L1094" s="10"/>
       <c r="M1094" s="40"/>
       <c r="N1094" s="37"/>
-      <c r="O1094" s="204" t="s">
+      <c r="O1094" s="202" t="s">
         <v>31</v>
       </c>
       <c r="P1094" s="10"/>
@@ -45151,8 +45178,8 @@
       <c r="L1095" s="52"/>
       <c r="M1095" s="54"/>
       <c r="N1095" s="55"/>
-      <c r="O1095" s="205" t="s">
-        <v>289</v>
+      <c r="O1095" s="203" t="s">
+        <v>288</v>
       </c>
       <c r="P1095" s="52"/>
       <c r="Q1095" s="57" t="s">
@@ -45304,7 +45331,7 @@
       <c r="L1099" s="30"/>
       <c r="M1099" s="80"/>
       <c r="N1099" s="37"/>
-      <c r="O1099" s="206">
+      <c r="O1099" s="204">
         <v>161</v>
       </c>
       <c r="P1099" s="10"/>
@@ -45345,7 +45372,7 @@
       <c r="L1100" s="30"/>
       <c r="M1100" s="80"/>
       <c r="N1100" s="37"/>
-      <c r="O1100" s="206">
+      <c r="O1100" s="204">
         <v>66</v>
       </c>
       <c r="P1100" s="10"/>
@@ -45386,7 +45413,7 @@
       <c r="L1101" s="30"/>
       <c r="M1101" s="80"/>
       <c r="N1101" s="37"/>
-      <c r="O1101" s="206">
+      <c r="O1101" s="204">
         <v>46</v>
       </c>
       <c r="P1101" s="10"/>
@@ -45423,8 +45450,8 @@
       <c r="L1102" s="10"/>
       <c r="M1102" s="40"/>
       <c r="N1102" s="37"/>
-      <c r="O1102" s="206" t="s">
-        <v>290</v>
+      <c r="O1102" s="204" t="s">
+        <v>289</v>
       </c>
       <c r="P1102" s="10"/>
       <c r="Q1102" s="44" t="s">
@@ -45462,7 +45489,7 @@
       <c r="L1103" s="10"/>
       <c r="M1103" s="40"/>
       <c r="N1103" s="37"/>
-      <c r="O1103" s="206"/>
+      <c r="O1103" s="204"/>
       <c r="P1103" s="10"/>
       <c r="Q1103" s="44" t="s">
         <v>15</v>
@@ -45499,8 +45526,8 @@
       <c r="L1104" s="10"/>
       <c r="M1104" s="40"/>
       <c r="N1104" s="37"/>
-      <c r="O1104" s="206" t="s">
-        <v>291</v>
+      <c r="O1104" s="204" t="s">
+        <v>290</v>
       </c>
       <c r="P1104" s="10"/>
       <c r="Q1104" s="44" t="s">
@@ -45538,7 +45565,7 @@
       <c r="L1105" s="10"/>
       <c r="M1105" s="40"/>
       <c r="N1105" s="37"/>
-      <c r="O1105" s="206" t="s">
+      <c r="O1105" s="204" t="s">
         <v>23</v>
       </c>
       <c r="P1105" s="10"/>
@@ -45577,8 +45604,8 @@
       <c r="L1106" s="10"/>
       <c r="M1106" s="40"/>
       <c r="N1106" s="37"/>
-      <c r="O1106" s="206" t="s">
-        <v>292</v>
+      <c r="O1106" s="204" t="s">
+        <v>291</v>
       </c>
       <c r="P1106" s="10"/>
       <c r="Q1106" s="44" t="s">
@@ -45616,8 +45643,8 @@
       <c r="L1107" s="10"/>
       <c r="M1107" s="40"/>
       <c r="N1107" s="37"/>
-      <c r="O1107" s="206" t="s">
-        <v>293</v>
+      <c r="O1107" s="204" t="s">
+        <v>292</v>
       </c>
       <c r="P1107" s="10"/>
       <c r="Q1107" s="44" t="s">
@@ -45655,8 +45682,8 @@
       <c r="L1108" s="52"/>
       <c r="M1108" s="54"/>
       <c r="N1108" s="55"/>
-      <c r="O1108" s="207" t="s">
-        <v>294</v>
+      <c r="O1108" s="205" t="s">
+        <v>293</v>
       </c>
       <c r="P1108" s="52"/>
       <c r="Q1108" s="57" t="s">
@@ -45808,7 +45835,7 @@
       <c r="L1112" s="30"/>
       <c r="M1112" s="80"/>
       <c r="N1112" s="37"/>
-      <c r="O1112" s="208">
+      <c r="O1112" s="206">
         <v>78</v>
       </c>
       <c r="P1112" s="10"/>
@@ -45849,7 +45876,7 @@
       <c r="L1113" s="30"/>
       <c r="M1113" s="80"/>
       <c r="N1113" s="37"/>
-      <c r="O1113" s="208">
+      <c r="O1113" s="206">
         <v>54</v>
       </c>
       <c r="P1113" s="10"/>
@@ -45890,7 +45917,7 @@
       <c r="L1114" s="30"/>
       <c r="M1114" s="80"/>
       <c r="N1114" s="37"/>
-      <c r="O1114" s="208">
+      <c r="O1114" s="206">
         <v>48</v>
       </c>
       <c r="P1114" s="10"/>
@@ -45927,8 +45954,8 @@
       <c r="L1115" s="10"/>
       <c r="M1115" s="40"/>
       <c r="N1115" s="37"/>
-      <c r="O1115" s="208" t="s">
-        <v>295</v>
+      <c r="O1115" s="206" t="s">
+        <v>294</v>
       </c>
       <c r="P1115" s="10"/>
       <c r="Q1115" s="44" t="s">
@@ -45966,8 +45993,8 @@
       <c r="L1116" s="10"/>
       <c r="M1116" s="40"/>
       <c r="N1116" s="37"/>
-      <c r="O1116" s="208" t="s">
-        <v>296</v>
+      <c r="O1116" s="206" t="s">
+        <v>295</v>
       </c>
       <c r="P1116" s="10"/>
       <c r="Q1116" s="44" t="s">
@@ -46005,8 +46032,8 @@
       <c r="L1117" s="10"/>
       <c r="M1117" s="40"/>
       <c r="N1117" s="37"/>
-      <c r="O1117" s="208" t="s">
-        <v>297</v>
+      <c r="O1117" s="206" t="s">
+        <v>296</v>
       </c>
       <c r="P1117" s="10"/>
       <c r="Q1117" s="44" t="s">
@@ -46044,7 +46071,7 @@
       <c r="L1118" s="10"/>
       <c r="M1118" s="40"/>
       <c r="N1118" s="37"/>
-      <c r="O1118" s="208" t="s">
+      <c r="O1118" s="206" t="s">
         <v>23</v>
       </c>
       <c r="P1118" s="10"/>
@@ -46083,7 +46110,7 @@
       <c r="L1119" s="10"/>
       <c r="M1119" s="40"/>
       <c r="N1119" s="37"/>
-      <c r="O1119" s="208" t="s">
+      <c r="O1119" s="206" t="s">
         <v>28</v>
       </c>
       <c r="P1119" s="10"/>
@@ -46122,7 +46149,7 @@
       <c r="L1120" s="10"/>
       <c r="M1120" s="40"/>
       <c r="N1120" s="37"/>
-      <c r="O1120" s="208" t="s">
+      <c r="O1120" s="206" t="s">
         <v>31</v>
       </c>
       <c r="P1120" s="10"/>
@@ -46161,8 +46188,8 @@
       <c r="L1121" s="52"/>
       <c r="M1121" s="54"/>
       <c r="N1121" s="55"/>
-      <c r="O1121" s="209" t="s">
-        <v>298</v>
+      <c r="O1121" s="207" t="s">
+        <v>297</v>
       </c>
       <c r="P1121" s="52"/>
       <c r="Q1121" s="57" t="s">
@@ -46314,7 +46341,7 @@
       <c r="L1125" s="30"/>
       <c r="M1125" s="80"/>
       <c r="N1125" s="37"/>
-      <c r="O1125" s="210">
+      <c r="O1125" s="208">
         <v>110</v>
       </c>
       <c r="P1125" s="10"/>
@@ -46355,7 +46382,7 @@
       <c r="L1126" s="30"/>
       <c r="M1126" s="80"/>
       <c r="N1126" s="37"/>
-      <c r="O1126" s="210">
+      <c r="O1126" s="208">
         <v>102</v>
       </c>
       <c r="P1126" s="10"/>
@@ -46396,7 +46423,7 @@
       <c r="L1127" s="30"/>
       <c r="M1127" s="80"/>
       <c r="N1127" s="37"/>
-      <c r="O1127" s="210">
+      <c r="O1127" s="208">
         <v>97</v>
       </c>
       <c r="P1127" s="10"/>
@@ -46433,8 +46460,8 @@
       <c r="L1128" s="10"/>
       <c r="M1128" s="40"/>
       <c r="N1128" s="37"/>
-      <c r="O1128" s="210" t="s">
-        <v>299</v>
+      <c r="O1128" s="208" t="s">
+        <v>298</v>
       </c>
       <c r="P1128" s="10"/>
       <c r="Q1128" s="44" t="s">
@@ -46472,7 +46499,7 @@
       <c r="L1129" s="10"/>
       <c r="M1129" s="40"/>
       <c r="N1129" s="37"/>
-      <c r="O1129" s="210"/>
+      <c r="O1129" s="208"/>
       <c r="P1129" s="10"/>
       <c r="Q1129" s="44" t="s">
         <v>15</v>
@@ -46509,8 +46536,8 @@
       <c r="L1130" s="10"/>
       <c r="M1130" s="40"/>
       <c r="N1130" s="37"/>
-      <c r="O1130" s="210" t="s">
-        <v>300</v>
+      <c r="O1130" s="208" t="s">
+        <v>299</v>
       </c>
       <c r="P1130" s="10"/>
       <c r="Q1130" s="44" t="s">
@@ -46548,7 +46575,7 @@
       <c r="L1131" s="10"/>
       <c r="M1131" s="40"/>
       <c r="N1131" s="37"/>
-      <c r="O1131" s="210" t="s">
+      <c r="O1131" s="208" t="s">
         <v>23</v>
       </c>
       <c r="P1131" s="10"/>
@@ -46587,7 +46614,7 @@
       <c r="L1132" s="10"/>
       <c r="M1132" s="40"/>
       <c r="N1132" s="37"/>
-      <c r="O1132" s="210" t="s">
+      <c r="O1132" s="208" t="s">
         <v>28</v>
       </c>
       <c r="P1132" s="10"/>
@@ -46626,7 +46653,7 @@
       <c r="L1133" s="10"/>
       <c r="M1133" s="40"/>
       <c r="N1133" s="37"/>
-      <c r="O1133" s="210" t="s">
+      <c r="O1133" s="208" t="s">
         <v>31</v>
       </c>
       <c r="P1133" s="10"/>
@@ -46665,8 +46692,8 @@
       <c r="L1134" s="52"/>
       <c r="M1134" s="54"/>
       <c r="N1134" s="55"/>
-      <c r="O1134" s="211" t="s">
-        <v>301</v>
+      <c r="O1134" s="209" t="s">
+        <v>300</v>
       </c>
       <c r="P1134" s="52"/>
       <c r="Q1134" s="57" t="s">
@@ -46818,7 +46845,7 @@
       <c r="L1138" s="30"/>
       <c r="M1138" s="80"/>
       <c r="N1138" s="37"/>
-      <c r="O1138" s="212">
+      <c r="O1138" s="210">
         <v>25</v>
       </c>
       <c r="P1138" s="10"/>
@@ -46859,7 +46886,7 @@
       <c r="L1139" s="30"/>
       <c r="M1139" s="80"/>
       <c r="N1139" s="37"/>
-      <c r="O1139" s="212">
+      <c r="O1139" s="210">
         <v>25</v>
       </c>
       <c r="P1139" s="10"/>
@@ -46900,7 +46927,7 @@
       <c r="L1140" s="30"/>
       <c r="M1140" s="80"/>
       <c r="N1140" s="37"/>
-      <c r="O1140" s="212">
+      <c r="O1140" s="210">
         <v>25</v>
       </c>
       <c r="P1140" s="10"/>
@@ -46937,8 +46964,8 @@
       <c r="L1141" s="10"/>
       <c r="M1141" s="40"/>
       <c r="N1141" s="37"/>
-      <c r="O1141" s="212" t="s">
-        <v>302</v>
+      <c r="O1141" s="210" t="s">
+        <v>301</v>
       </c>
       <c r="P1141" s="10"/>
       <c r="Q1141" s="44" t="s">
@@ -46976,8 +47003,8 @@
       <c r="L1142" s="10"/>
       <c r="M1142" s="40"/>
       <c r="N1142" s="37"/>
-      <c r="O1142" s="212" t="s">
-        <v>303</v>
+      <c r="O1142" s="210" t="s">
+        <v>302</v>
       </c>
       <c r="P1142" s="10"/>
       <c r="Q1142" s="44" t="s">
@@ -47015,8 +47042,8 @@
       <c r="L1143" s="10"/>
       <c r="M1143" s="40"/>
       <c r="N1143" s="37"/>
-      <c r="O1143" s="212" t="s">
-        <v>304</v>
+      <c r="O1143" s="210" t="s">
+        <v>303</v>
       </c>
       <c r="P1143" s="10"/>
       <c r="Q1143" s="44" t="s">
@@ -47054,7 +47081,7 @@
       <c r="L1144" s="10"/>
       <c r="M1144" s="40"/>
       <c r="N1144" s="37"/>
-      <c r="O1144" s="212" t="s">
+      <c r="O1144" s="210" t="s">
         <v>23</v>
       </c>
       <c r="P1144" s="10"/>
@@ -47093,7 +47120,7 @@
       <c r="L1145" s="10"/>
       <c r="M1145" s="40"/>
       <c r="N1145" s="37"/>
-      <c r="O1145" s="212" t="s">
+      <c r="O1145" s="210" t="s">
         <v>28</v>
       </c>
       <c r="P1145" s="10"/>
@@ -47132,7 +47159,7 @@
       <c r="L1146" s="10"/>
       <c r="M1146" s="40"/>
       <c r="N1146" s="37"/>
-      <c r="O1146" s="212" t="s">
+      <c r="O1146" s="210" t="s">
         <v>31</v>
       </c>
       <c r="P1146" s="10"/>
@@ -47171,8 +47198,8 @@
       <c r="L1147" s="52"/>
       <c r="M1147" s="54"/>
       <c r="N1147" s="55"/>
-      <c r="O1147" s="213" t="s">
-        <v>305</v>
+      <c r="O1147" s="211" t="s">
+        <v>304</v>
       </c>
       <c r="P1147" s="52"/>
       <c r="Q1147" s="57" t="s">
@@ -47324,7 +47351,7 @@
       <c r="L1151" s="30"/>
       <c r="M1151" s="80"/>
       <c r="N1151" s="37"/>
-      <c r="O1151" s="214">
+      <c r="O1151" s="212">
         <v>0</v>
       </c>
       <c r="P1151" s="10"/>
@@ -47365,7 +47392,7 @@
       <c r="L1152" s="30"/>
       <c r="M1152" s="80"/>
       <c r="N1152" s="37"/>
-      <c r="O1152" s="214">
+      <c r="O1152" s="212">
         <v>0</v>
       </c>
       <c r="P1152" s="10"/>
@@ -47406,7 +47433,7 @@
       <c r="L1153" s="30"/>
       <c r="M1153" s="80"/>
       <c r="N1153" s="37"/>
-      <c r="O1153" s="214">
+      <c r="O1153" s="212">
         <v>0</v>
       </c>
       <c r="P1153" s="10"/>
@@ -47443,7 +47470,7 @@
       <c r="L1154" s="10"/>
       <c r="M1154" s="40"/>
       <c r="N1154" s="37"/>
-      <c r="O1154" s="214" t="s">
+      <c r="O1154" s="212" t="s">
         <v>120</v>
       </c>
       <c r="P1154" s="10"/>
@@ -47482,7 +47509,7 @@
       <c r="L1155" s="10"/>
       <c r="M1155" s="40"/>
       <c r="N1155" s="37"/>
-      <c r="O1155" s="214"/>
+      <c r="O1155" s="212"/>
       <c r="P1155" s="10"/>
       <c r="Q1155" s="44" t="s">
         <v>15</v>
@@ -47519,8 +47546,8 @@
       <c r="L1156" s="10"/>
       <c r="M1156" s="40"/>
       <c r="N1156" s="37"/>
-      <c r="O1156" s="214" t="s">
-        <v>307</v>
+      <c r="O1156" s="212" t="s">
+        <v>306</v>
       </c>
       <c r="P1156" s="10"/>
       <c r="Q1156" s="44" t="s">
@@ -47558,8 +47585,8 @@
       <c r="L1157" s="10"/>
       <c r="M1157" s="40"/>
       <c r="N1157" s="37"/>
-      <c r="O1157" s="214" t="s">
-        <v>309</v>
+      <c r="O1157" s="212" t="s">
+        <v>308</v>
       </c>
       <c r="P1157" s="10"/>
       <c r="Q1157" s="44" t="s">
@@ -47597,8 +47624,8 @@
       <c r="L1158" s="10"/>
       <c r="M1158" s="40"/>
       <c r="N1158" s="37"/>
-      <c r="O1158" s="214" t="s">
-        <v>308</v>
+      <c r="O1158" s="212" t="s">
+        <v>307</v>
       </c>
       <c r="P1158" s="10"/>
       <c r="Q1158" s="44" t="s">
@@ -47636,8 +47663,8 @@
       <c r="L1159" s="10"/>
       <c r="M1159" s="40"/>
       <c r="N1159" s="37"/>
-      <c r="O1159" s="214" t="s">
-        <v>308</v>
+      <c r="O1159" s="212" t="s">
+        <v>307</v>
       </c>
       <c r="P1159" s="10"/>
       <c r="Q1159" s="44" t="s">
@@ -47675,8 +47702,8 @@
       <c r="L1160" s="52"/>
       <c r="M1160" s="54"/>
       <c r="N1160" s="55"/>
-      <c r="O1160" s="215" t="s">
-        <v>306</v>
+      <c r="O1160" s="213" t="s">
+        <v>305</v>
       </c>
       <c r="P1160" s="52"/>
       <c r="Q1160" s="57" t="s">
@@ -47828,7 +47855,7 @@
       <c r="L1164" s="30"/>
       <c r="M1164" s="80"/>
       <c r="N1164" s="37"/>
-      <c r="O1164" s="216">
+      <c r="O1164" s="214">
         <v>255</v>
       </c>
       <c r="P1164" s="10"/>
@@ -47869,7 +47896,7 @@
       <c r="L1165" s="30"/>
       <c r="M1165" s="80"/>
       <c r="N1165" s="37"/>
-      <c r="O1165" s="216">
+      <c r="O1165" s="214">
         <v>255</v>
       </c>
       <c r="P1165" s="10"/>
@@ -47910,7 +47937,7 @@
       <c r="L1166" s="30"/>
       <c r="M1166" s="80"/>
       <c r="N1166" s="37"/>
-      <c r="O1166" s="216">
+      <c r="O1166" s="214">
         <v>255</v>
       </c>
       <c r="P1166" s="10"/>
@@ -47947,8 +47974,8 @@
       <c r="L1167" s="10"/>
       <c r="M1167" s="40"/>
       <c r="N1167" s="37"/>
-      <c r="O1167" s="216" t="s">
-        <v>310</v>
+      <c r="O1167" s="214" t="s">
+        <v>309</v>
       </c>
       <c r="P1167" s="10"/>
       <c r="Q1167" s="44" t="s">
@@ -47986,8 +48013,8 @@
       <c r="L1168" s="10"/>
       <c r="M1168" s="40"/>
       <c r="N1168" s="37"/>
-      <c r="O1168" s="216" t="s">
-        <v>313</v>
+      <c r="O1168" s="214" t="s">
+        <v>312</v>
       </c>
       <c r="P1168" s="10"/>
       <c r="Q1168" s="44" t="s">
@@ -48025,8 +48052,8 @@
       <c r="L1169" s="10"/>
       <c r="M1169" s="40"/>
       <c r="N1169" s="37"/>
-      <c r="O1169" s="216" t="s">
-        <v>311</v>
+      <c r="O1169" s="214" t="s">
+        <v>310</v>
       </c>
       <c r="P1169" s="10"/>
       <c r="Q1169" s="44" t="s">
@@ -48064,8 +48091,8 @@
       <c r="L1170" s="10"/>
       <c r="M1170" s="40"/>
       <c r="N1170" s="37"/>
-      <c r="O1170" s="216" t="s">
-        <v>314</v>
+      <c r="O1170" s="214" t="s">
+        <v>313</v>
       </c>
       <c r="P1170" s="10"/>
       <c r="Q1170" s="44" t="s">
@@ -48103,8 +48130,8 @@
       <c r="L1171" s="10"/>
       <c r="M1171" s="40"/>
       <c r="N1171" s="37"/>
-      <c r="O1171" s="216" t="s">
-        <v>308</v>
+      <c r="O1171" s="214" t="s">
+        <v>307</v>
       </c>
       <c r="P1171" s="10"/>
       <c r="Q1171" s="44" t="s">
@@ -48142,8 +48169,8 @@
       <c r="L1172" s="10"/>
       <c r="M1172" s="40"/>
       <c r="N1172" s="37"/>
-      <c r="O1172" s="216" t="s">
-        <v>308</v>
+      <c r="O1172" s="214" t="s">
+        <v>307</v>
       </c>
       <c r="P1172" s="10"/>
       <c r="Q1172" s="44" t="s">
@@ -48181,8 +48208,8 @@
       <c r="L1173" s="52"/>
       <c r="M1173" s="54"/>
       <c r="N1173" s="55"/>
-      <c r="O1173" s="217" t="s">
-        <v>312</v>
+      <c r="O1173" s="215" t="s">
+        <v>311</v>
       </c>
       <c r="P1173" s="52"/>
       <c r="Q1173" s="57" t="s">
@@ -48334,7 +48361,7 @@
       <c r="L1177" s="30"/>
       <c r="M1177" s="80"/>
       <c r="N1177" s="37"/>
-      <c r="O1177" s="218">
+      <c r="O1177" s="216">
         <v>110</v>
       </c>
       <c r="P1177" s="10"/>
@@ -48375,7 +48402,7 @@
       <c r="L1178" s="30"/>
       <c r="M1178" s="80"/>
       <c r="N1178" s="37"/>
-      <c r="O1178" s="218">
+      <c r="O1178" s="216">
         <v>90</v>
       </c>
       <c r="P1178" s="10"/>
@@ -48416,7 +48443,7 @@
       <c r="L1179" s="30"/>
       <c r="M1179" s="80"/>
       <c r="N1179" s="37"/>
-      <c r="O1179" s="218">
+      <c r="O1179" s="216">
         <v>154</v>
       </c>
       <c r="P1179" s="10"/>
@@ -48453,8 +48480,8 @@
       <c r="L1180" s="10"/>
       <c r="M1180" s="40"/>
       <c r="N1180" s="37"/>
-      <c r="O1180" s="218" t="s">
-        <v>315</v>
+      <c r="O1180" s="216" t="s">
+        <v>314</v>
       </c>
       <c r="P1180" s="10"/>
       <c r="Q1180" s="44" t="s">
@@ -48492,7 +48519,7 @@
       <c r="L1181" s="10"/>
       <c r="M1181" s="40"/>
       <c r="N1181" s="37"/>
-      <c r="O1181" s="218"/>
+      <c r="O1181" s="216"/>
       <c r="P1181" s="10"/>
       <c r="Q1181" s="44" t="s">
         <v>15</v>
@@ -48529,8 +48556,8 @@
       <c r="L1182" s="10"/>
       <c r="M1182" s="40"/>
       <c r="N1182" s="37"/>
-      <c r="O1182" s="218" t="s">
-        <v>316</v>
+      <c r="O1182" s="216" t="s">
+        <v>315</v>
       </c>
       <c r="P1182" s="10"/>
       <c r="Q1182" s="44" t="s">
@@ -48568,7 +48595,7 @@
       <c r="L1183" s="10"/>
       <c r="M1183" s="40"/>
       <c r="N1183" s="37"/>
-      <c r="O1183" s="218" t="s">
+      <c r="O1183" s="216" t="s">
         <v>23</v>
       </c>
       <c r="P1183" s="10"/>
@@ -48607,8 +48634,8 @@
       <c r="L1184" s="10"/>
       <c r="M1184" s="40"/>
       <c r="N1184" s="37"/>
-      <c r="O1184" s="218" t="s">
-        <v>246</v>
+      <c r="O1184" s="216" t="s">
+        <v>245</v>
       </c>
       <c r="P1184" s="10"/>
       <c r="Q1184" s="44" t="s">
@@ -48646,8 +48673,8 @@
       <c r="L1185" s="10"/>
       <c r="M1185" s="40"/>
       <c r="N1185" s="37"/>
-      <c r="O1185" s="218" t="s">
-        <v>208</v>
+      <c r="O1185" s="216" t="s">
+        <v>207</v>
       </c>
       <c r="P1185" s="10"/>
       <c r="Q1185" s="44" t="s">
@@ -48685,8 +48712,8 @@
       <c r="L1186" s="52"/>
       <c r="M1186" s="54"/>
       <c r="N1186" s="55"/>
-      <c r="O1186" s="219" t="s">
-        <v>317</v>
+      <c r="O1186" s="217" t="s">
+        <v>316</v>
       </c>
       <c r="P1186" s="52"/>
       <c r="Q1186" s="57" t="s">
@@ -48838,7 +48865,7 @@
       <c r="L1190" s="30"/>
       <c r="M1190" s="80"/>
       <c r="N1190" s="37"/>
-      <c r="O1190" s="214">
+      <c r="O1190" s="212">
         <v>0</v>
       </c>
       <c r="P1190" s="10"/>
@@ -48879,7 +48906,7 @@
       <c r="L1191" s="30"/>
       <c r="M1191" s="80"/>
       <c r="N1191" s="37"/>
-      <c r="O1191" s="214">
+      <c r="O1191" s="212">
         <v>0</v>
       </c>
       <c r="P1191" s="10"/>
@@ -48920,7 +48947,7 @@
       <c r="L1192" s="30"/>
       <c r="M1192" s="80"/>
       <c r="N1192" s="37"/>
-      <c r="O1192" s="214">
+      <c r="O1192" s="212">
         <v>0</v>
       </c>
       <c r="P1192" s="10"/>
@@ -48957,7 +48984,7 @@
       <c r="L1193" s="10"/>
       <c r="M1193" s="40"/>
       <c r="N1193" s="37"/>
-      <c r="O1193" s="214" t="s">
+      <c r="O1193" s="212" t="s">
         <v>120</v>
       </c>
       <c r="P1193" s="10"/>
@@ -48996,8 +49023,8 @@
       <c r="L1194" s="10"/>
       <c r="M1194" s="40"/>
       <c r="N1194" s="37"/>
-      <c r="O1194" s="214" t="s">
-        <v>303</v>
+      <c r="O1194" s="212" t="s">
+        <v>302</v>
       </c>
       <c r="P1194" s="10"/>
       <c r="Q1194" s="44" t="s">
@@ -49035,8 +49062,8 @@
       <c r="L1195" s="10"/>
       <c r="M1195" s="40"/>
       <c r="N1195" s="37"/>
-      <c r="O1195" s="214" t="s">
-        <v>318</v>
+      <c r="O1195" s="212" t="s">
+        <v>317</v>
       </c>
       <c r="P1195" s="10"/>
       <c r="Q1195" s="44" t="s">
@@ -49074,8 +49101,8 @@
       <c r="L1196" s="10"/>
       <c r="M1196" s="40"/>
       <c r="N1196" s="37"/>
-      <c r="O1196" s="214" t="s">
-        <v>319</v>
+      <c r="O1196" s="212" t="s">
+        <v>318</v>
       </c>
       <c r="P1196" s="10"/>
       <c r="Q1196" s="44" t="s">
@@ -49113,8 +49140,8 @@
       <c r="L1197" s="10"/>
       <c r="M1197" s="40"/>
       <c r="N1197" s="37"/>
-      <c r="O1197" s="214" t="s">
-        <v>320</v>
+      <c r="O1197" s="212" t="s">
+        <v>319</v>
       </c>
       <c r="P1197" s="10"/>
       <c r="Q1197" s="44" t="s">
@@ -49152,8 +49179,8 @@
       <c r="L1198" s="10"/>
       <c r="M1198" s="40"/>
       <c r="N1198" s="37"/>
-      <c r="O1198" s="214" t="s">
-        <v>320</v>
+      <c r="O1198" s="212" t="s">
+        <v>319</v>
       </c>
       <c r="P1198" s="10"/>
       <c r="Q1198" s="44" t="s">
@@ -49191,8 +49218,8 @@
       <c r="L1199" s="52"/>
       <c r="M1199" s="54"/>
       <c r="N1199" s="55"/>
-      <c r="O1199" s="215" t="s">
-        <v>321</v>
+      <c r="O1199" s="213" t="s">
+        <v>320</v>
       </c>
       <c r="P1199" s="52"/>
       <c r="Q1199" s="57" t="s">
@@ -49344,7 +49371,7 @@
       <c r="L1203" s="30"/>
       <c r="M1203" s="80"/>
       <c r="N1203" s="37"/>
-      <c r="O1203" s="220">
+      <c r="O1203" s="218">
         <v>255</v>
       </c>
       <c r="P1203" s="10"/>
@@ -49385,7 +49412,7 @@
       <c r="L1204" s="30"/>
       <c r="M1204" s="80"/>
       <c r="N1204" s="37"/>
-      <c r="O1204" s="220">
+      <c r="O1204" s="218">
         <v>255</v>
       </c>
       <c r="P1204" s="10"/>
@@ -49426,7 +49453,7 @@
       <c r="L1205" s="30"/>
       <c r="M1205" s="80"/>
       <c r="N1205" s="37"/>
-      <c r="O1205" s="220">
+      <c r="O1205" s="218">
         <v>255</v>
       </c>
       <c r="P1205" s="10"/>
@@ -49463,7 +49490,7 @@
       <c r="L1206" s="10"/>
       <c r="M1206" s="40"/>
       <c r="N1206" s="37"/>
-      <c r="O1206" s="220" t="s">
+      <c r="O1206" s="218" t="s">
         <v>166</v>
       </c>
       <c r="P1206" s="10"/>
@@ -49502,7 +49529,7 @@
       <c r="L1207" s="10"/>
       <c r="M1207" s="40"/>
       <c r="N1207" s="37"/>
-      <c r="O1207" s="220"/>
+      <c r="O1207" s="218"/>
       <c r="P1207" s="10"/>
       <c r="Q1207" s="44" t="s">
         <v>15</v>
@@ -49539,8 +49566,8 @@
       <c r="L1208" s="10"/>
       <c r="M1208" s="40"/>
       <c r="N1208" s="37"/>
-      <c r="O1208" s="220" t="s">
-        <v>322</v>
+      <c r="O1208" s="218" t="s">
+        <v>321</v>
       </c>
       <c r="P1208" s="10"/>
       <c r="Q1208" s="44" t="s">
@@ -49578,7 +49605,7 @@
       <c r="L1209" s="10"/>
       <c r="M1209" s="40"/>
       <c r="N1209" s="37"/>
-      <c r="O1209" s="220" t="s">
+      <c r="O1209" s="218" t="s">
         <v>23</v>
       </c>
       <c r="P1209" s="10"/>
@@ -49617,8 +49644,8 @@
       <c r="L1210" s="10"/>
       <c r="M1210" s="40"/>
       <c r="N1210" s="37"/>
-      <c r="O1210" s="220" t="s">
-        <v>206</v>
+      <c r="O1210" s="218" t="s">
+        <v>205</v>
       </c>
       <c r="P1210" s="10"/>
       <c r="Q1210" s="44" t="s">
@@ -49656,8 +49683,8 @@
       <c r="L1211" s="10"/>
       <c r="M1211" s="40"/>
       <c r="N1211" s="37"/>
-      <c r="O1211" s="220" t="s">
-        <v>208</v>
+      <c r="O1211" s="218" t="s">
+        <v>207</v>
       </c>
       <c r="P1211" s="10"/>
       <c r="Q1211" s="44" t="s">
@@ -49695,8 +49722,8 @@
       <c r="L1212" s="52"/>
       <c r="M1212" s="54"/>
       <c r="N1212" s="55"/>
-      <c r="O1212" s="221" t="s">
-        <v>323</v>
+      <c r="O1212" s="219" t="s">
+        <v>322</v>
       </c>
       <c r="P1212" s="52"/>
       <c r="Q1212" s="57" t="s">
@@ -49848,7 +49875,7 @@
       <c r="L1216" s="30"/>
       <c r="M1216" s="80"/>
       <c r="N1216" s="37"/>
-      <c r="O1216" s="214">
+      <c r="O1216" s="212">
         <v>0</v>
       </c>
       <c r="P1216" s="10"/>
@@ -49889,7 +49916,7 @@
       <c r="L1217" s="30"/>
       <c r="M1217" s="80"/>
       <c r="N1217" s="37"/>
-      <c r="O1217" s="214">
+      <c r="O1217" s="212">
         <v>0</v>
       </c>
       <c r="P1217" s="10"/>
@@ -49930,7 +49957,7 @@
       <c r="L1218" s="30"/>
       <c r="M1218" s="80"/>
       <c r="N1218" s="37"/>
-      <c r="O1218" s="214">
+      <c r="O1218" s="212">
         <v>0</v>
       </c>
       <c r="P1218" s="10"/>
@@ -49967,7 +49994,7 @@
       <c r="L1219" s="10"/>
       <c r="M1219" s="40"/>
       <c r="N1219" s="37"/>
-      <c r="O1219" s="214" t="s">
+      <c r="O1219" s="212" t="s">
         <v>120</v>
       </c>
       <c r="P1219" s="10"/>
@@ -50006,7 +50033,7 @@
       <c r="L1220" s="10"/>
       <c r="M1220" s="40"/>
       <c r="N1220" s="37"/>
-      <c r="O1220" s="214" t="s">
+      <c r="O1220" s="212" t="s">
         <v>121</v>
       </c>
       <c r="P1220" s="10"/>
@@ -50045,7 +50072,7 @@
       <c r="L1221" s="10"/>
       <c r="M1221" s="40"/>
       <c r="N1221" s="37"/>
-      <c r="O1221" s="214"/>
+      <c r="O1221" s="212"/>
       <c r="P1221" s="10"/>
       <c r="Q1221" s="44" t="s">
         <v>15</v>
@@ -50082,7 +50109,7 @@
       <c r="L1222" s="10"/>
       <c r="M1222" s="40"/>
       <c r="N1222" s="37"/>
-      <c r="O1222" s="214" t="s">
+      <c r="O1222" s="212" t="s">
         <v>122</v>
       </c>
       <c r="P1222" s="10"/>
@@ -50121,8 +50148,8 @@
       <c r="L1223" s="10"/>
       <c r="M1223" s="40"/>
       <c r="N1223" s="37"/>
-      <c r="O1223" s="214" t="s">
-        <v>324</v>
+      <c r="O1223" s="212" t="s">
+        <v>323</v>
       </c>
       <c r="P1223" s="10"/>
       <c r="Q1223" s="44" t="s">
@@ -50160,7 +50187,7 @@
       <c r="L1224" s="10"/>
       <c r="M1224" s="40"/>
       <c r="N1224" s="37"/>
-      <c r="O1224" s="214" t="s">
+      <c r="O1224" s="212" t="s">
         <v>124</v>
       </c>
       <c r="P1224" s="10"/>
@@ -50199,8 +50226,8 @@
       <c r="L1225" s="52"/>
       <c r="M1225" s="54"/>
       <c r="N1225" s="55"/>
-      <c r="O1225" s="215" t="s">
-        <v>325</v>
+      <c r="O1225" s="213" t="s">
+        <v>324</v>
       </c>
       <c r="P1225" s="52"/>
       <c r="Q1225" s="57" t="s">
@@ -50352,7 +50379,7 @@
       <c r="L1229" s="30"/>
       <c r="M1229" s="80"/>
       <c r="N1229" s="37"/>
-      <c r="O1229" s="168">
+      <c r="O1229" s="166">
         <v>249</v>
       </c>
       <c r="P1229" s="10"/>
@@ -50393,7 +50420,7 @@
       <c r="L1230" s="30"/>
       <c r="M1230" s="80"/>
       <c r="N1230" s="37"/>
-      <c r="O1230" s="168">
+      <c r="O1230" s="166">
         <v>249</v>
       </c>
       <c r="P1230" s="10"/>
@@ -50434,7 +50461,7 @@
       <c r="L1231" s="30"/>
       <c r="M1231" s="80"/>
       <c r="N1231" s="37"/>
-      <c r="O1231" s="168">
+      <c r="O1231" s="166">
         <v>249</v>
       </c>
       <c r="P1231" s="10"/>
@@ -50471,7 +50498,7 @@
       <c r="L1232" s="10"/>
       <c r="M1232" s="40"/>
       <c r="N1232" s="37"/>
-      <c r="O1232" s="168"/>
+      <c r="O1232" s="166"/>
       <c r="P1232" s="10"/>
       <c r="Q1232" s="44" t="s">
         <v>15</v>
@@ -50508,7 +50535,7 @@
       <c r="L1233" s="10"/>
       <c r="M1233" s="40"/>
       <c r="N1233" s="37"/>
-      <c r="O1233" s="168"/>
+      <c r="O1233" s="166"/>
       <c r="P1233" s="10"/>
       <c r="Q1233" s="44" t="s">
         <v>15</v>
@@ -50545,7 +50572,7 @@
       <c r="L1234" s="10"/>
       <c r="M1234" s="40"/>
       <c r="N1234" s="37"/>
-      <c r="O1234" s="168"/>
+      <c r="O1234" s="166"/>
       <c r="P1234" s="10"/>
       <c r="Q1234" s="44" t="s">
         <v>15</v>
@@ -50582,7 +50609,7 @@
       <c r="L1235" s="10"/>
       <c r="M1235" s="40"/>
       <c r="N1235" s="37"/>
-      <c r="O1235" s="168"/>
+      <c r="O1235" s="166"/>
       <c r="P1235" s="10"/>
       <c r="Q1235" s="44" t="s">
         <v>15</v>
@@ -50619,7 +50646,7 @@
       <c r="L1236" s="10"/>
       <c r="M1236" s="40"/>
       <c r="N1236" s="37"/>
-      <c r="O1236" s="168"/>
+      <c r="O1236" s="166"/>
       <c r="P1236" s="10"/>
       <c r="Q1236" s="44" t="s">
         <v>15</v>
@@ -50656,7 +50683,7 @@
       <c r="L1237" s="10"/>
       <c r="M1237" s="40"/>
       <c r="N1237" s="37"/>
-      <c r="O1237" s="168"/>
+      <c r="O1237" s="166"/>
       <c r="P1237" s="10"/>
       <c r="Q1237" s="44" t="s">
         <v>15</v>
@@ -50693,7 +50720,7 @@
       <c r="L1238" s="52"/>
       <c r="M1238" s="54"/>
       <c r="N1238" s="55"/>
-      <c r="O1238" s="169"/>
+      <c r="O1238" s="167"/>
       <c r="P1238" s="52"/>
       <c r="Q1238" s="57" t="s">
         <v>15</v>
@@ -50844,7 +50871,7 @@
       <c r="L1242" s="30"/>
       <c r="M1242" s="80"/>
       <c r="N1242" s="37"/>
-      <c r="O1242" s="168">
+      <c r="O1242" s="166">
         <v>249</v>
       </c>
       <c r="P1242" s="10"/>
@@ -50885,7 +50912,7 @@
       <c r="L1243" s="30"/>
       <c r="M1243" s="80"/>
       <c r="N1243" s="37"/>
-      <c r="O1243" s="168">
+      <c r="O1243" s="166">
         <v>249</v>
       </c>
       <c r="P1243" s="10"/>
@@ -50926,7 +50953,7 @@
       <c r="L1244" s="30"/>
       <c r="M1244" s="80"/>
       <c r="N1244" s="37"/>
-      <c r="O1244" s="168">
+      <c r="O1244" s="166">
         <v>249</v>
       </c>
       <c r="P1244" s="10"/>
@@ -50963,7 +50990,7 @@
       <c r="L1245" s="10"/>
       <c r="M1245" s="40"/>
       <c r="N1245" s="37"/>
-      <c r="O1245" s="168"/>
+      <c r="O1245" s="166"/>
       <c r="P1245" s="10"/>
       <c r="Q1245" s="44" t="s">
         <v>15</v>
@@ -51000,7 +51027,7 @@
       <c r="L1246" s="10"/>
       <c r="M1246" s="40"/>
       <c r="N1246" s="37"/>
-      <c r="O1246" s="168"/>
+      <c r="O1246" s="166"/>
       <c r="P1246" s="10"/>
       <c r="Q1246" s="44" t="s">
         <v>15</v>
@@ -51037,7 +51064,7 @@
       <c r="L1247" s="10"/>
       <c r="M1247" s="40"/>
       <c r="N1247" s="37"/>
-      <c r="O1247" s="168"/>
+      <c r="O1247" s="166"/>
       <c r="P1247" s="10"/>
       <c r="Q1247" s="44" t="s">
         <v>15</v>
@@ -51074,7 +51101,7 @@
       <c r="L1248" s="10"/>
       <c r="M1248" s="40"/>
       <c r="N1248" s="37"/>
-      <c r="O1248" s="168"/>
+      <c r="O1248" s="166"/>
       <c r="P1248" s="10"/>
       <c r="Q1248" s="44" t="s">
         <v>15</v>
@@ -51111,7 +51138,7 @@
       <c r="L1249" s="10"/>
       <c r="M1249" s="40"/>
       <c r="N1249" s="37"/>
-      <c r="O1249" s="168"/>
+      <c r="O1249" s="166"/>
       <c r="P1249" s="10"/>
       <c r="Q1249" s="44" t="s">
         <v>15</v>
@@ -51148,7 +51175,7 @@
       <c r="L1250" s="10"/>
       <c r="M1250" s="40"/>
       <c r="N1250" s="37"/>
-      <c r="O1250" s="168"/>
+      <c r="O1250" s="166"/>
       <c r="P1250" s="10"/>
       <c r="Q1250" s="44" t="s">
         <v>15</v>
@@ -51185,7 +51212,7 @@
       <c r="L1251" s="52"/>
       <c r="M1251" s="54"/>
       <c r="N1251" s="55"/>
-      <c r="O1251" s="169"/>
+      <c r="O1251" s="167"/>
       <c r="P1251" s="52"/>
       <c r="Q1251" s="57" t="s">
         <v>15</v>
@@ -51336,7 +51363,7 @@
       <c r="L1255" s="30"/>
       <c r="M1255" s="80"/>
       <c r="N1255" s="37"/>
-      <c r="O1255" s="168">
+      <c r="O1255" s="166">
         <v>249</v>
       </c>
       <c r="P1255" s="10"/>
@@ -51377,7 +51404,7 @@
       <c r="L1256" s="30"/>
       <c r="M1256" s="80"/>
       <c r="N1256" s="37"/>
-      <c r="O1256" s="168">
+      <c r="O1256" s="166">
         <v>249</v>
       </c>
       <c r="P1256" s="10"/>
@@ -51418,7 +51445,7 @@
       <c r="L1257" s="30"/>
       <c r="M1257" s="80"/>
       <c r="N1257" s="37"/>
-      <c r="O1257" s="168">
+      <c r="O1257" s="166">
         <v>249</v>
       </c>
       <c r="P1257" s="10"/>
@@ -51455,7 +51482,7 @@
       <c r="L1258" s="10"/>
       <c r="M1258" s="40"/>
       <c r="N1258" s="37"/>
-      <c r="O1258" s="168"/>
+      <c r="O1258" s="166"/>
       <c r="P1258" s="10"/>
       <c r="Q1258" s="44" t="s">
         <v>15</v>
@@ -51492,7 +51519,7 @@
       <c r="L1259" s="10"/>
       <c r="M1259" s="40"/>
       <c r="N1259" s="37"/>
-      <c r="O1259" s="168"/>
+      <c r="O1259" s="166"/>
       <c r="P1259" s="10"/>
       <c r="Q1259" s="44" t="s">
         <v>15</v>
@@ -51529,7 +51556,7 @@
       <c r="L1260" s="10"/>
       <c r="M1260" s="40"/>
       <c r="N1260" s="37"/>
-      <c r="O1260" s="168"/>
+      <c r="O1260" s="166"/>
       <c r="P1260" s="10"/>
       <c r="Q1260" s="44" t="s">
         <v>15</v>
@@ -51566,7 +51593,7 @@
       <c r="L1261" s="10"/>
       <c r="M1261" s="40"/>
       <c r="N1261" s="37"/>
-      <c r="O1261" s="168"/>
+      <c r="O1261" s="166"/>
       <c r="P1261" s="10"/>
       <c r="Q1261" s="44" t="s">
         <v>15</v>
@@ -51603,7 +51630,7 @@
       <c r="L1262" s="10"/>
       <c r="M1262" s="40"/>
       <c r="N1262" s="37"/>
-      <c r="O1262" s="168"/>
+      <c r="O1262" s="166"/>
       <c r="P1262" s="10"/>
       <c r="Q1262" s="44" t="s">
         <v>15</v>
@@ -51640,7 +51667,7 @@
       <c r="L1263" s="10"/>
       <c r="M1263" s="40"/>
       <c r="N1263" s="37"/>
-      <c r="O1263" s="168"/>
+      <c r="O1263" s="166"/>
       <c r="P1263" s="10"/>
       <c r="Q1263" s="44" t="s">
         <v>15</v>
@@ -51677,7 +51704,7 @@
       <c r="L1264" s="52"/>
       <c r="M1264" s="54"/>
       <c r="N1264" s="55"/>
-      <c r="O1264" s="169"/>
+      <c r="O1264" s="167"/>
       <c r="P1264" s="52"/>
       <c r="Q1264" s="57" t="s">
         <v>15</v>
@@ -51828,7 +51855,7 @@
       <c r="L1268" s="30"/>
       <c r="M1268" s="80"/>
       <c r="N1268" s="37"/>
-      <c r="O1268" s="168">
+      <c r="O1268" s="166">
         <v>249</v>
       </c>
       <c r="P1268" s="10"/>
@@ -51869,7 +51896,7 @@
       <c r="L1269" s="30"/>
       <c r="M1269" s="80"/>
       <c r="N1269" s="37"/>
-      <c r="O1269" s="168">
+      <c r="O1269" s="166">
         <v>249</v>
       </c>
       <c r="P1269" s="10"/>
@@ -51910,7 +51937,7 @@
       <c r="L1270" s="30"/>
       <c r="M1270" s="80"/>
       <c r="N1270" s="37"/>
-      <c r="O1270" s="168">
+      <c r="O1270" s="166">
         <v>249</v>
       </c>
       <c r="P1270" s="10"/>
@@ -51947,7 +51974,7 @@
       <c r="L1271" s="10"/>
       <c r="M1271" s="40"/>
       <c r="N1271" s="37"/>
-      <c r="O1271" s="168"/>
+      <c r="O1271" s="166"/>
       <c r="P1271" s="10"/>
       <c r="Q1271" s="44" t="s">
         <v>15</v>
@@ -51984,7 +52011,7 @@
       <c r="L1272" s="10"/>
       <c r="M1272" s="40"/>
       <c r="N1272" s="37"/>
-      <c r="O1272" s="168"/>
+      <c r="O1272" s="166"/>
       <c r="P1272" s="10"/>
       <c r="Q1272" s="44" t="s">
         <v>15</v>
@@ -52021,7 +52048,7 @@
       <c r="L1273" s="10"/>
       <c r="M1273" s="40"/>
       <c r="N1273" s="37"/>
-      <c r="O1273" s="168"/>
+      <c r="O1273" s="166"/>
       <c r="P1273" s="10"/>
       <c r="Q1273" s="44" t="s">
         <v>15</v>
@@ -52058,7 +52085,7 @@
       <c r="L1274" s="10"/>
       <c r="M1274" s="40"/>
       <c r="N1274" s="37"/>
-      <c r="O1274" s="168"/>
+      <c r="O1274" s="166"/>
       <c r="P1274" s="10"/>
       <c r="Q1274" s="44" t="s">
         <v>15</v>
@@ -52095,7 +52122,7 @@
       <c r="L1275" s="10"/>
       <c r="M1275" s="40"/>
       <c r="N1275" s="37"/>
-      <c r="O1275" s="168"/>
+      <c r="O1275" s="166"/>
       <c r="P1275" s="10"/>
       <c r="Q1275" s="44" t="s">
         <v>15</v>
@@ -52132,7 +52159,7 @@
       <c r="L1276" s="10"/>
       <c r="M1276" s="40"/>
       <c r="N1276" s="37"/>
-      <c r="O1276" s="168"/>
+      <c r="O1276" s="166"/>
       <c r="P1276" s="10"/>
       <c r="Q1276" s="44" t="s">
         <v>15</v>
@@ -52169,7 +52196,7 @@
       <c r="L1277" s="52"/>
       <c r="M1277" s="54"/>
       <c r="N1277" s="55"/>
-      <c r="O1277" s="169"/>
+      <c r="O1277" s="167"/>
       <c r="P1277" s="52"/>
       <c r="Q1277" s="57" t="s">
         <v>15</v>
@@ -52320,7 +52347,7 @@
       <c r="L1281" s="30"/>
       <c r="M1281" s="80"/>
       <c r="N1281" s="37"/>
-      <c r="O1281" s="168">
+      <c r="O1281" s="166">
         <v>249</v>
       </c>
       <c r="P1281" s="10"/>
@@ -52361,7 +52388,7 @@
       <c r="L1282" s="30"/>
       <c r="M1282" s="80"/>
       <c r="N1282" s="37"/>
-      <c r="O1282" s="168">
+      <c r="O1282" s="166">
         <v>249</v>
       </c>
       <c r="P1282" s="10"/>
@@ -52402,7 +52429,7 @@
       <c r="L1283" s="30"/>
       <c r="M1283" s="80"/>
       <c r="N1283" s="37"/>
-      <c r="O1283" s="168">
+      <c r="O1283" s="166">
         <v>249</v>
       </c>
       <c r="P1283" s="10"/>
@@ -52439,7 +52466,7 @@
       <c r="L1284" s="10"/>
       <c r="M1284" s="40"/>
       <c r="N1284" s="37"/>
-      <c r="O1284" s="168"/>
+      <c r="O1284" s="166"/>
       <c r="P1284" s="10"/>
       <c r="Q1284" s="44" t="s">
         <v>15</v>
@@ -52476,7 +52503,7 @@
       <c r="L1285" s="10"/>
       <c r="M1285" s="40"/>
       <c r="N1285" s="37"/>
-      <c r="O1285" s="168"/>
+      <c r="O1285" s="166"/>
       <c r="P1285" s="10"/>
       <c r="Q1285" s="44" t="s">
         <v>15</v>
@@ -52513,7 +52540,7 @@
       <c r="L1286" s="10"/>
       <c r="M1286" s="40"/>
       <c r="N1286" s="37"/>
-      <c r="O1286" s="168"/>
+      <c r="O1286" s="166"/>
       <c r="P1286" s="10"/>
       <c r="Q1286" s="44" t="s">
         <v>15</v>
@@ -52550,7 +52577,7 @@
       <c r="L1287" s="10"/>
       <c r="M1287" s="40"/>
       <c r="N1287" s="37"/>
-      <c r="O1287" s="168"/>
+      <c r="O1287" s="166"/>
       <c r="P1287" s="10"/>
       <c r="Q1287" s="44" t="s">
         <v>15</v>
@@ -52587,7 +52614,7 @@
       <c r="L1288" s="10"/>
       <c r="M1288" s="40"/>
       <c r="N1288" s="37"/>
-      <c r="O1288" s="168"/>
+      <c r="O1288" s="166"/>
       <c r="P1288" s="10"/>
       <c r="Q1288" s="44" t="s">
         <v>15</v>
@@ -52624,7 +52651,7 @@
       <c r="L1289" s="10"/>
       <c r="M1289" s="40"/>
       <c r="N1289" s="37"/>
-      <c r="O1289" s="168"/>
+      <c r="O1289" s="166"/>
       <c r="P1289" s="10"/>
       <c r="Q1289" s="44" t="s">
         <v>15</v>
@@ -52661,7 +52688,7 @@
       <c r="L1290" s="52"/>
       <c r="M1290" s="54"/>
       <c r="N1290" s="55"/>
-      <c r="O1290" s="169"/>
+      <c r="O1290" s="167"/>
       <c r="P1290" s="52"/>
       <c r="Q1290" s="57" t="s">
         <v>15</v>
@@ -52684,9 +52711,9 @@
       <c r="K1291" s="41"/>
       <c r="L1291" s="30"/>
       <c r="M1291" s="40"/>
-      <c r="N1291" s="222"/>
+      <c r="N1291" s="220"/>
       <c r="O1291" s="38"/>
-      <c r="P1291" s="223"/>
+      <c r="P1291" s="221"/>
       <c r="Q1291" s="43"/>
       <c r="R1291" s="27"/>
     </row>
@@ -52704,9 +52731,9 @@
       <c r="K1292" s="41"/>
       <c r="L1292" s="30"/>
       <c r="M1292" s="40"/>
-      <c r="N1292" s="222"/>
+      <c r="N1292" s="220"/>
       <c r="O1292" s="38"/>
-      <c r="P1292" s="223"/>
+      <c r="P1292" s="221"/>
       <c r="Q1292" s="43"/>
       <c r="R1292" s="27"/>
     </row>
@@ -52724,9 +52751,9 @@
       <c r="K1293" s="41"/>
       <c r="L1293" s="30"/>
       <c r="M1293" s="40"/>
-      <c r="N1293" s="222"/>
+      <c r="N1293" s="220"/>
       <c r="O1293" s="38"/>
-      <c r="P1293" s="223"/>
+      <c r="P1293" s="221"/>
       <c r="Q1293" s="43"/>
       <c r="R1293" s="27"/>
     </row>
@@ -52744,14 +52771,14 @@
       <c r="K1294" s="41"/>
       <c r="L1294" s="30"/>
       <c r="M1294" s="40"/>
-      <c r="N1294" s="222"/>
+      <c r="N1294" s="220"/>
       <c r="O1294" s="38"/>
-      <c r="P1294" s="223"/>
+      <c r="P1294" s="221"/>
       <c r="Q1294" s="43"/>
       <c r="R1294" s="27"/>
     </row>
     <row r="1295" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1295" s="224"/>
+      <c r="A1295" s="222"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>